<commit_message>
تحديث الملف: 9/27/2025, 3:38:07 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1223"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -439,7 +439,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ما هو التعريف الأدق لل COPD</v>
+        <v>ما و التعريف الأدق لل COPD</v>
       </c>
       <c r="B2" t="str">
         <v>التهاب فيروس حاد للرئة</v>
@@ -4847,7 +4847,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" xml:space="preserve">
+    <row r="128">
       <c r="A128" t="str">
         <v>رجل عمره 70 سنة لديه داء سكري ومدخن الضغط في ذراعه اليمنى 80/180 واليسرى 75/100</v>
       </c>
@@ -4869,16 +4869,8 @@
       <c r="G128" t="str">
         <v>5</v>
       </c>
-      <c r="H128" t="str" xml:space="preserve">
-        <v xml:space="preserve">تم أضافة شرح فقط: هلق هون ممكن معو تضيق عصيدي بالطرف الايسر فضغطه عم ينخفض باليسار_x000d_
-فهون عندو يعني اعتلال اوعية وافضل خافض ضغط بهالحالة هنن حاصرات كالسيوم_x000d_
-_x000d_
-او عندو تسلخ ابهر فعم يصير فرق بين الطرفين_x000d_
-هون العلاج هو لابيتالول اللي هو حاصر بيتا_x000d_
-وممكن علاج جراحي حسب نوع التسلخ_x000d_
-_x000d_
-بقا حسب اش بدو الدكتور واش قصدو_x000d_
-غالبا الحالة الاولى لانو ما ذكر الم صدري او شي الو علاقة بالتسلخ</v>
+      <c r="H128" t="str">
+        <v>تم أضافة شرح فقط: هلق هون ممكن معو تضيق عصيدي بالطرف الايسر فضغطه عم ينخفض باليسار_x000d_فهون عندو يعني اعتلال اوعية وافضل خافض ضغط بهالحالة هنن حاصرات كالسيوم_x000d__x000d_او عندو تسلخ ابهر فعم يصير فرق بين الطرفين_x000d_هون العلاج هو لابيتالول اللي هو حاصر بيتا_x000d_وممكن علاج جراحي حسب نوع التسلخ_x000d__x000d_بقا حسب اش بدو الدكتور واش قصدو_x000d_غالبا الحالة الاولى لانو ما ذكر الم صدري او شي الو علاقة بالتسلخ</v>
       </c>
       <c r="I128" t="str">
         <v>داخلية قلبية</v>
@@ -4890,7 +4882,7 @@
         <v>تصويبات</v>
       </c>
     </row>
-    <row r="129" xml:space="preserve">
+    <row r="129">
       <c r="A129" t="str">
         <v>امرأة عمرها 53 سنة لديها نوب متكرر من الصداع والتوهج وضغطها اثناء نوبة الصداع 95/155 مع نبض 92 خارج نوبة الصداع 75/115</v>
       </c>
@@ -4912,11 +4904,8 @@
       <c r="G129" t="str">
         <v>5</v>
       </c>
-      <c r="H129" t="str" xml:space="preserve">
-        <v xml:space="preserve">تم اضافة شرح فقط: معا ورم قواتم_x000d_
-افضل علاج دوائي هو حاصرات الفا_x000d_
-او جراحة_x000d_
-الصداع ناتج عن تقبض الاوعية الدماغية استجابة للضغط المرتفع</v>
+      <c r="H129" t="str">
+        <v>تم اضافة شرح فقط: معا ورم قواتم_x000d_افضل علاج دوائي هو حاصرات الفا_x000d_او جراحة_x000d_الصداع ناتج عن تقبض الاوعية الدماغية استجابة للضغط المرتفع</v>
       </c>
       <c r="I129" t="str">
         <v>داخلية قلبية</v>
@@ -24633,16 +24622,15 @@
         <v/>
       </c>
     </row>
-    <row r="693" xml:space="preserve">
+    <row r="693">
       <c r="A693" t="str">
         <v>فيما يتعلق ب FAST كل مما يلي صحيح ماعدا:</v>
       </c>
       <c r="B693" t="str">
         <v>وسيلة استقصائية</v>
       </c>
-      <c r="C693" t="str" xml:space="preserve">
-        <v xml:space="preserve">وسيلة سريعة_x000d_
-</v>
+      <c r="C693" t="str">
+        <v>وسيلة سريعة_x000d_</v>
       </c>
       <c r="D693" t="str">
         <v>تستخدم لتقييم الحصيات المرارية</v>

</xml_diff>

<commit_message>
تحديث الملف: 9/27/2025, 3:42:55 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -439,7 +439,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ما و التعريف الأدق لل COPD</v>
+        <v>ما هو التعريف الأدق لل COPD</v>
       </c>
       <c r="B2" t="str">
         <v>التهاب فيروس حاد للرئة</v>
@@ -460,7 +460,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>🔥</v>
       </c>
       <c r="I2" t="str">
         <v>داخلية صدرية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/27/2025, 10:51:08 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -439,7 +439,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ما هو التعريف الأدق لل COPD</v>
+        <v>ما هو التعريف الأدق لل COPD:</v>
       </c>
       <c r="B2" t="str">
         <v>التهاب فيروس حاد للرئة</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>ماهو التظاهر المرضي المميز للشكل الوراثي من ‎(COPD)‏ المرتبط بعوز الالفا- ‎١‏ انتيتريبسين:‌‏</v>
+        <v>ماهو التظاهر المرضي المميز للشكل الوراثي من ‎(COPD)‏ المرتبط بعوز الالفا- ‎1 انتيتريبسين:‌‏</v>
       </c>
       <c r="B6" t="str">
         <v>انتفاخ رئوي قاعدي</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/27/2025, 2:34:30 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -3085,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="H77" t="str">
-        <v/>
+        <v>رباعي فالو شنت ايمن - ايسر اما الباقي كلن ايسر-ايمن</v>
       </c>
       <c r="I77" t="str">
         <v>داخلية قلبية</v>
@@ -3120,7 +3120,7 @@
         <v>5</v>
       </c>
       <c r="H78" t="str">
-        <v/>
+        <v>تم إضافة شرح فقط: اخترنا الخيار الصحيح،  ASD اشيع لدى الاناث</v>
       </c>
       <c r="I78" t="str">
         <v>داخلية قلبية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/27/2025, 3:03:15 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -2945,7 +2945,7 @@
         <v>4</v>
       </c>
       <c r="H73" t="str">
-        <v/>
+        <v>الكوليسترول عامل خطر للتصلب العصيدي وليس للضغط</v>
       </c>
       <c r="I73" t="str">
         <v>داخلية قلبية</v>
@@ -3015,7 +3015,7 @@
         <v>5</v>
       </c>
       <c r="H75" t="str">
-        <v/>
+        <v>العلاج جراحي</v>
       </c>
       <c r="I75" t="str">
         <v>داخلية قلبية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 27/09/2025, 16:15:34
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -3799,7 +3799,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>يتميز قصور القلب الحاد الأيسر (وذنة الرئة الحادة)</v>
+        <v>يتميز قصور القلب الحاد الأيسر (وذمة الرئة الحادة)</v>
       </c>
       <c r="B98" t="str">
         <v>ارتفاع الضغط داخل البطين الأيمن في نهاية الانبساط</v>
@@ -3855,7 +3855,7 @@
         <v>2</v>
       </c>
       <c r="H99" t="str">
-        <v/>
+        <v>المدرات لا تزيد البقيا</v>
       </c>
       <c r="I99" t="str">
         <v>داخلية قلبية</v>
@@ -3925,7 +3925,7 @@
         <v>3</v>
       </c>
       <c r="H101" t="str">
-        <v/>
+        <v>من مدرات العروة امثلة اخرى: فورسمايد-Bumetanide</v>
       </c>
       <c r="I101" t="str">
         <v>داخلية قلبية</v>
@@ -4590,7 +4590,7 @@
         <v>5</v>
       </c>
       <c r="H120" t="str">
-        <v/>
+        <v>ارتفاع الانزيمات القلبية</v>
       </c>
       <c r="I120" t="str">
         <v>داخلية قلبية</v>
@@ -4625,7 +4625,7 @@
         <v>2</v>
       </c>
       <c r="H121" t="str">
-        <v/>
+        <v>اخترنا الصح، الظليل ادق،يجب ان يكون القلب بطيء، يتم ايقاف التنفس 6-7ث</v>
       </c>
       <c r="I121" t="str">
         <v>داخلية قلبية</v>
@@ -4969,10 +4969,10 @@
         <v>تبديل الصمام التاجي أفضل من تصنيعه</v>
       </c>
       <c r="F131" t="str">
-        <v/>
+        <v>الديجوكسين يفيد في المعالجة إذا كانت نسبة المقذوف اقل من 45% وخاصة المترافق بالرجفان الاذيني</v>
       </c>
       <c r="G131" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H131" t="str">
         <v/>
@@ -4984,7 +4984,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K131" t="str">
-        <v/>
+        <v>تصويبات</v>
       </c>
     </row>
     <row r="132">
@@ -5339,7 +5339,7 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>امرأة عمرها 70 سنة تشتكتي من زلة تنفسية على الجهود المتوسطة: لديها قصة ارتفاع توتر شرياني قديم: تخطيط القلب أظهر ضخامة بطين أيسر الايكو EF: 60% ماهو التشخيص الأكثر احتمالا</v>
+        <v>امرأة عمرها 70 سنة تشتكي من زلة تنفسية على الجهود المتوسطة: لديها قصة ارتفاع توتر شرياني قديم: تخطيط القلب أظهر ضخامة بطين أيسر الايكو EF: 60% ماهو التشخيص الأكثر احتمالا</v>
       </c>
       <c r="B142" t="str">
         <v>قصور قلب انبساطي</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 1:19:05 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -18800,7 +18800,7 @@
         <v>5</v>
       </c>
       <c r="H526" t="str">
-        <v/>
+        <v>4_5 kg</v>
       </c>
       <c r="I526" t="str">
         <v>جلدية</v>
@@ -18835,7 +18835,7 @@
         <v>1</v>
       </c>
       <c r="H527" t="str">
-        <v/>
+        <v>فوق الطبقة القاعدية</v>
       </c>
       <c r="I527" t="str">
         <v>جلدية</v>
@@ -18870,7 +18870,7 @@
         <v>4</v>
       </c>
       <c r="H528" t="str">
-        <v/>
+        <v>الخلايا الكيراتينية</v>
       </c>
       <c r="I528" t="str">
         <v>جلدية</v>
@@ -18882,7 +18882,7 @@
         <v/>
       </c>
     </row>
-    <row r="529">
+    <row r="529" xml:space="preserve">
       <c r="A529" t="str">
         <v>أي ممايلي صحيح عن الطبقة المتقرنة</v>
       </c>
@@ -18904,8 +18904,14 @@
       <c r="G529" t="str">
         <v>2</v>
       </c>
-      <c r="H529" t="str">
-        <v/>
+      <c r="H529" t="str" xml:space="preserve">
+        <v xml:space="preserve">الطبقة المتقرنة (Stratum Corneum)
+· عدد طبقات الخلايا المطسحة: من 15 إلى 20 طبقة (وقد تصل إلى 100 طبقة في باطن اليد والقدم).
+· حجم وأنوية الخلايا: لا تحتوي على أنوية. الخلايا ميتة ومسطحة.
+· مكانها في الجسم: أعلى طبقة في البشرة، وتوجد في جميع أنحاء الجسم، لكن سماكتها تختلف حسب المنطقة.
+· السماكة: رقيقة في معظم المناطق (مثل الجفن)، وسميكة جدًا في مناطق الاحتكاك (مثل باطن اليد والقدم).
+· المكونات: خلايا كيراتينية ميتة (مليئة بالكيراتين) مغطاة بطبقة شحمية.
+· الإفرازات: لا تفرز أي شيء.</v>
       </c>
       <c r="I529" t="str">
         <v>جلدية</v>
@@ -18917,7 +18923,7 @@
         <v/>
       </c>
     </row>
-    <row r="530">
+    <row r="530" xml:space="preserve">
       <c r="A530" t="str">
         <v>أي ممايلي صحيح عن الطبقة القاعدية:</v>
       </c>
@@ -18939,8 +18945,12 @@
       <c r="G530" t="str">
         <v>1</v>
       </c>
-      <c r="H530" t="str">
-        <v/>
+      <c r="H530" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+· الحد الفاصل: الأدمة (وليس الطبقة القاعدية) هي التي تفصل البشرة عن النسيج تحت الجلد.
+· عدد الصفوف: الطبقة القاعدية تتكون من صف واحد فقط من الخلايا.
+· خلايا لانغرهانس: توجد في الطبقة الشوكية وليس في القاعدية.
+· الطبقة السطحية: الطبقة السطحية للبشرة هي الطبقة المتقرنة وليست القاعدية.</v>
       </c>
       <c r="I530" t="str">
         <v>جلدية</v>
@@ -18975,7 +18985,7 @@
         <v>4</v>
       </c>
       <c r="H531" t="str">
-        <v/>
+        <v>لا تحوي نسيج شحمي</v>
       </c>
       <c r="I531" t="str">
         <v>جلدية</v>
@@ -19010,7 +19020,7 @@
         <v>2</v>
       </c>
       <c r="H532" t="str">
-        <v/>
+        <v>حطاطات مقببة</v>
       </c>
       <c r="I532" t="str">
         <v>جلدية</v>
@@ -19045,7 +19055,7 @@
         <v>5</v>
       </c>
       <c r="H533" t="str">
-        <v/>
+        <v>مؤلم عرضه المميز</v>
       </c>
       <c r="I533" t="str">
         <v>جلدية</v>
@@ -19057,7 +19067,7 @@
         <v/>
       </c>
     </row>
-    <row r="534">
+    <row r="534" xml:space="preserve">
       <c r="A534" t="str">
         <v>ناتج جفاف مفرزات مصلية أو قيحية أو دموية:</v>
       </c>
@@ -19079,8 +19089,11 @@
       <c r="G534" t="str">
         <v>2</v>
       </c>
-      <c r="H534" t="str">
-        <v/>
+      <c r="H534" t="str" xml:space="preserve">
+        <v xml:space="preserve">سحجة: خدش سطحي للجلد.
+تآكل: فقدان الطبقة السطحية من الجلد أو الغشاء المخاطي.
+تقرح: فقدان أعمق للأنسجة يصل إلى ما تحت الأدمة.
+تحزز: تشقق في الجلد.</v>
       </c>
       <c r="I534" t="str">
         <v>جلدية</v>
@@ -19092,7 +19105,7 @@
         <v/>
       </c>
     </row>
-    <row r="535">
+    <row r="535" xml:space="preserve">
       <c r="A535" t="str">
         <v>تجمع مصلي بقطر أقل من 0.5 سم:</v>
       </c>
@@ -19114,8 +19127,11 @@
       <c r="G535" t="str">
         <v>3</v>
       </c>
-      <c r="H535" t="str">
-        <v/>
+      <c r="H535" t="str" xml:space="preserve">
+        <v xml:space="preserve">حطاطة: نتوء صلب صغير بدون رأس (أقل من 1 سم).
+عقيدة: نتوء صلب أكبر من الحطاطة (أكبر من 1 سم).
+فقاعة: انتفاخ يحتوي على سائل مائي صافي (أكبر من 1 سم).
+بثرة: انتفاخ صغير يحتوي على صديد (قيح).</v>
       </c>
       <c r="I535" t="str">
         <v>جلدية</v>
@@ -19127,7 +19143,7 @@
         <v/>
       </c>
     </row>
-    <row r="536">
+    <row r="536" xml:space="preserve">
       <c r="A536" t="str">
         <v>مايلي صحيح عن الشعر ماعدا:</v>
       </c>
@@ -19149,8 +19165,13 @@
       <c r="G536" t="str">
         <v>4</v>
       </c>
-      <c r="H536" t="str">
-        <v/>
+      <c r="H536" t="str" xml:space="preserve">
+        <v xml:space="preserve">ايضا لا ينمو على  راحتي اليدين
+أخمص القدمين
+الشفتين
+الحلمتين
+الندوب
+الأغشية المخاطية</v>
       </c>
       <c r="I536" t="str">
         <v>جلدية</v>
@@ -19185,7 +19206,7 @@
         <v>4</v>
       </c>
       <c r="H537" t="str">
-        <v/>
+        <v>سريعة الانتشار بالتلامس او الاجسام</v>
       </c>
       <c r="I537" t="str">
         <v>جلدية</v>
@@ -19197,7 +19218,7 @@
         <v/>
       </c>
     </row>
-    <row r="538">
+    <row r="538" xml:space="preserve">
       <c r="A538" t="str">
         <v>أي مما يلي صحيح عن الدمل:</v>
       </c>
@@ -19219,8 +19240,12 @@
       <c r="G538" t="str">
         <v>1</v>
       </c>
-      <c r="H538" t="str">
-        <v/>
+      <c r="H538" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+· المسبب: المكور العنقودي الذهبي (وليس الزوائف).
+· الألم: يكون مؤلمًا (وليس غير مؤلم).
+· الندبة: قد يخلف ندبة بعد الشفاء (وليس دائمًا بدون ندبة).
+· المكان: لا يظهر في الراحتين والأخمصين (لأنها عديمة البصيلات).</v>
       </c>
       <c r="I538" t="str">
         <v>جلدية</v>
@@ -19232,7 +19257,7 @@
         <v/>
       </c>
     </row>
-    <row r="539">
+    <row r="539" xml:space="preserve">
       <c r="A539" t="str">
         <v>مايلي صحيح عن القوباء ماعدا:</v>
       </c>
@@ -19254,8 +19279,10 @@
       <c r="G539" t="str">
         <v>5</v>
       </c>
-      <c r="H539" t="str">
-        <v/>
+      <c r="H539" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+القوباء مرض معدٍ بشدة.
+· طريقة الانتقال: التلامس المباشر مع القروح أو السائل الذي يخرج منها، أو عن طريق الأدوات الملوثة (مثل المناشف).</v>
       </c>
       <c r="I539" t="str">
         <v>جلدية</v>
@@ -19267,7 +19294,7 @@
         <v/>
       </c>
     </row>
-    <row r="540">
+    <row r="540" xml:space="preserve">
       <c r="A540" t="str">
         <v>المرض الذي يسبب نز قيحي من الإحليل:</v>
       </c>
@@ -19289,8 +19316,13 @@
       <c r="G540" t="str">
         <v>3</v>
       </c>
-      <c r="H540" t="str">
-        <v/>
+      <c r="H540" t="str" xml:space="preserve">
+        <v xml:space="preserve">المرض الذي يسبب نز قيحي من الإحليل هو السيلان البني (Gonorrhea).
+أما الأمراض الأخرى فتُسبب أعراضاً مختلفة في أماكن أخرى:
+· السفلس (الزهري): يسبب قرحة صلبة غير مؤلمة (شانكر) في مكان دخول العدوى.
+· الحبيبوم الإربي: يسبب تقرحات وتورماً مؤلماً في العقد الليمفاوية الإربية.
+· الحبيبوم الليني: يسبب تقرحات جلدية متدرجة في المنطقة الإربية والتناسلية.
+· القريح: يسبب قرحة تناسلية مؤلمة وتقرحاً في العقد الليمفاوية.</v>
       </c>
       <c r="I540" t="str">
         <v>جلدية</v>
@@ -19302,7 +19334,7 @@
         <v/>
       </c>
     </row>
-    <row r="541">
+    <row r="541" xml:space="preserve">
       <c r="A541" t="str">
         <v>الوسوف البيضاء الفضية الغزيرة مميزة لـ:</v>
       </c>
@@ -19324,8 +19356,12 @@
       <c r="G541" t="str">
         <v>4</v>
       </c>
-      <c r="H541" t="str">
-        <v/>
+      <c r="H541" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+· الحزاز المسطح: حطاطات أرجوانية مسطحة ذات سطح لامع.
+· البهق: بقع بيضاء حليبية (خالية تمامًا من الصباغ) ذات حواف واضحة.
+· المهق: افتقاد كامل لصباغ الجلد والشعر والعينين منذ الولادة.
+· صلابة الجلد: تصلب وشد في الجلد يصاحبه تغير في اللون.</v>
       </c>
       <c r="I541" t="str">
         <v>جلدية</v>
@@ -19337,7 +19373,7 @@
         <v/>
       </c>
     </row>
-    <row r="542">
+    <row r="542" xml:space="preserve">
       <c r="A542" t="str">
         <v>مايلي صحيح عن التهاب الغدد العرقية المقيح ما عدا:</v>
       </c>
@@ -19359,8 +19395,10 @@
       <c r="G542" t="str">
         <v>4</v>
       </c>
-      <c r="H542" t="str">
-        <v/>
+      <c r="H542" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+التهاب الغدد العرقية القيحي (Hidradenitis Suppurativa) هو مرض ناكس (مزمن ومتكرر).
+· الناكس: يتميز بفترات من هجوع المرض تتبعها نوبات متكررة من ظهور الدمامل والالتهابات في مناطق ثنايا الجلد.</v>
       </c>
       <c r="I542" t="str">
         <v>جلدية</v>
@@ -19395,7 +19433,7 @@
         <v>1</v>
       </c>
       <c r="H543" t="str">
-        <v/>
+        <v>المزمن سببه فطري  مبيضات بيض</v>
       </c>
       <c r="I543" t="str">
         <v>جلدية</v>
@@ -19430,7 +19468,7 @@
         <v>3</v>
       </c>
       <c r="H544" t="str">
-        <v/>
+        <v>العقديات بشكل شائع A واحيانا G</v>
       </c>
       <c r="I544" t="str">
         <v>جلدية</v>
@@ -19465,7 +19503,7 @@
         <v>3</v>
       </c>
       <c r="H545" t="str">
-        <v/>
+        <v>علامة نيكولسكي إيجابية: حيث يؤدي فرك الجلد بلطف إلى تقشره.</v>
       </c>
       <c r="I545" t="str">
         <v>جلدية</v>
@@ -19500,7 +19538,7 @@
         <v>5</v>
       </c>
       <c r="H546" t="str">
-        <v/>
+        <v>بل يسبب تقعر اظافر</v>
       </c>
       <c r="I546" t="str">
         <v>جلدية</v>
@@ -19512,7 +19550,7 @@
         <v/>
       </c>
     </row>
-    <row r="547">
+    <row r="547" xml:space="preserve">
       <c r="A547" t="str">
         <v>الاجراء الأفضل لتشخيص التهاب الجلد التماسي:</v>
       </c>
@@ -19534,8 +19572,10 @@
       <c r="G547" t="str">
         <v>4</v>
       </c>
-      <c r="H547" t="str">
-        <v/>
+      <c r="H547" t="str" xml:space="preserve">
+        <v xml:space="preserve">التهاب الجلد التماسي هو طفح جلدي أحمر مثير للحكة يحدث عندما يلمس الجلد مادة مهيجة أو مسببة للحساسية.
+علاقته باختبار الرقعة:
+يستخدم اختبار الرقعة لتشخيص السبب، حيث يتم وضع لصقات تحتوي على مواد شائعة مسببة للحساسية على الجلد لمدة 48 ساعة، ثم فحص المنطقة بعد 48-96 ساعة لاكتشاف أي رد فعل تحسسي.</v>
       </c>
       <c r="I547" t="str">
         <v>جلدية</v>
@@ -19547,7 +19587,7 @@
         <v/>
       </c>
     </row>
-    <row r="548">
+    <row r="548" xml:space="preserve">
       <c r="A548" t="str">
         <v>مرض يتسبب عن النمط الثاني للتفاعلات الأرجية (التفاعل السام للخلايا):</v>
       </c>
@@ -19569,8 +19609,11 @@
       <c r="G548" t="str">
         <v>3</v>
       </c>
-      <c r="H548" t="str">
-        <v/>
+      <c r="H548" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+· الصدمة التأقية والشري: النمط الأول.
+· التهاب الأوعية: النمط الثالث.
+· التهاب الجلد التماسي: النمط الرابع.</v>
       </c>
       <c r="I548" t="str">
         <v>جلدية</v>
@@ -19605,7 +19648,7 @@
         <v>2</v>
       </c>
       <c r="H549" t="str">
-        <v/>
+        <v>تنتج الذيفان المسؤول عن انحلال الطبقة الخارجية من الجلد وتشكل الفقاعات.</v>
       </c>
       <c r="I549" t="str">
         <v>جلدية</v>
@@ -19640,7 +19683,7 @@
         <v>2</v>
       </c>
       <c r="H550" t="str">
-        <v/>
+        <v>المرتبط بسرطان عنق الرحم هو فيروس الورم الحليمي البشري (HPV)، وليس فيروس الحلأ البسيط (HSV).</v>
       </c>
       <c r="I550" t="str">
         <v>جلدية</v>
@@ -19675,7 +19718,7 @@
         <v>2</v>
       </c>
       <c r="H551" t="str">
-        <v/>
+        <v>تزداد مع تقدم العمر</v>
       </c>
       <c r="I551" t="str">
         <v>جلدية</v>
@@ -19710,7 +19753,7 @@
         <v>4</v>
       </c>
       <c r="H552" t="str">
-        <v/>
+        <v>الذئبة الشائعة(SLE) هو مرض مناعة ذاتية جهازي وليس شكلاً من أشكال السل الجلدي.</v>
       </c>
       <c r="I552" t="str">
         <v>جلدية</v>
@@ -19745,7 +19788,7 @@
         <v>1</v>
       </c>
       <c r="H553" t="str">
-        <v/>
+        <v>ويُستخدم الحقن لآفات التهابية وليس تقرني مثل الثاليل</v>
       </c>
       <c r="I553" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 1:22:47 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -19870,7 +19870,7 @@
         <v/>
       </c>
     </row>
-    <row r="556">
+    <row r="556" xml:space="preserve">
       <c r="A556" t="str">
         <v>أي مما يلي سرطانة لابدة داخل البشرة carcinoma in situ</v>
       </c>
@@ -19892,8 +19892,9 @@
       <c r="G556" t="str">
         <v>5</v>
       </c>
-      <c r="H556" t="str">
-        <v/>
+      <c r="H556" t="str" xml:space="preserve">
+        <v xml:space="preserve">البُهاق:
+مرض مناعي مكتسب يتميز بظهور بقع بيضاء (خالية تمامًا من صبغة الميلانين) على الجلد، ذات حواف واضحة، بسبب تدمير الخلايا الصبغية.</v>
       </c>
       <c r="I556" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 1:23:43 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -19906,7 +19906,7 @@
         <v/>
       </c>
     </row>
-    <row r="557">
+    <row r="557" xml:space="preserve">
       <c r="A557" t="str">
         <v>أي مما يلي صحيح عن الحماق</v>
       </c>
@@ -19928,8 +19928,11 @@
       <c r="G557" t="str">
         <v>5</v>
       </c>
-      <c r="H557" t="str">
-        <v/>
+      <c r="H557" t="str" xml:space="preserve">
+        <v xml:space="preserve">داء بوفن هو الاسم التاريخي لمرض يُعرف اليوم باسم:
+الورم الحليمي البشري (HPV) - Human Papilloma Virus
+المقصود تحديداً: الإصابة بفيروس الورم الحليمي البشري في منطقة الأعضاء التناسلية والشرج، والتي تسبب ظهور ثآليل تناسلية (Condylomata acuminata).
+الاسم الحديث الشائع لهذا المظهر السريري هو: "الورم اللقمي" أو "الثآليل التناسلية".</v>
       </c>
       <c r="I557" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 1:24:48 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -19944,7 +19944,7 @@
         <v/>
       </c>
     </row>
-    <row r="558">
+    <row r="558" xml:space="preserve">
       <c r="A558" t="str">
         <v>مايلي صحيح عن الثاليل الشائعة ما عدا:</v>
       </c>
@@ -19966,8 +19966,12 @@
       <c r="G558" t="str">
         <v>4</v>
       </c>
-      <c r="H558" t="str">
-        <v/>
+      <c r="H558" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+· المرض يكون عرضياً بوضوح.
+· يصيب الأطفال بشكل رئيسي.
+· قد يؤدي إلى مضاعفات في بعض الحالات.
+· العرض الرئيسي هو حكة جلدية شديدة.</v>
       </c>
       <c r="I558" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 1:41:07 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -19835,7 +19835,7 @@
         <v/>
       </c>
     </row>
-    <row r="555">
+    <row r="555" xml:space="preserve">
       <c r="A555" t="str">
         <v>إمراضية البهاق:</v>
       </c>
@@ -19857,8 +19857,9 @@
       <c r="G555" t="str">
         <v>4</v>
       </c>
-      <c r="H555" t="str">
-        <v/>
+      <c r="H555" t="str" xml:space="preserve">
+        <v xml:space="preserve">البُهاق:
+مرض مناعي مكتسب يتميز بظهور بقع بيضاء (خالية تمامًا من صبغة الميلانين) على الجلد، ذات حواف واضحة، بسبب تدمير الخلايا الصبغية.</v>
       </c>
       <c r="I555" t="str">
         <v>جلدية</v>
@@ -19893,86 +19894,85 @@
         <v>5</v>
       </c>
       <c r="H556" t="str" xml:space="preserve">
-        <v xml:space="preserve">البُهاق:
-مرض مناعي مكتسب يتميز بظهور بقع بيضاء (خالية تمامًا من صبغة الميلانين) على الجلد، ذات حواف واضحة، بسبب تدمير الخلايا الصبغية.</v>
-      </c>
-      <c r="I556" t="str">
-        <v>جلدية</v>
-      </c>
-      <c r="J556" t="str">
-        <v>الفصل الثاني 2024-2025</v>
-      </c>
-      <c r="K556" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="557" xml:space="preserve">
-      <c r="A557" t="str">
-        <v>أي مما يلي صحيح عن الحماق</v>
-      </c>
-      <c r="B557" t="str">
-        <v>الإصابة غير عرضية</v>
-      </c>
-      <c r="C557" t="str">
-        <v>يصيب البالغين عادة</v>
-      </c>
-      <c r="D557" t="str">
-        <v>يبقى الفيروس كامناً في الجسم بعد الإصابة</v>
-      </c>
-      <c r="E557" t="str">
-        <v>ليس له أية اختلاطات</v>
-      </c>
-      <c r="F557" t="str">
-        <v>الإصابة مؤلمة</v>
-      </c>
-      <c r="G557" t="str">
-        <v>5</v>
-      </c>
-      <c r="H557" t="str" xml:space="preserve">
         <v xml:space="preserve">داء بوفن هو الاسم التاريخي لمرض يُعرف اليوم باسم:
 الورم الحليمي البشري (HPV) - Human Papilloma Virus
 المقصود تحديداً: الإصابة بفيروس الورم الحليمي البشري في منطقة الأعضاء التناسلية والشرج، والتي تسبب ظهور ثآليل تناسلية (Condylomata acuminata).
 الاسم الحديث الشائع لهذا المظهر السريري هو: "الورم اللقمي" أو "الثآليل التناسلية".</v>
       </c>
-      <c r="I557" t="str">
+      <c r="I556" t="str">
         <v>جلدية</v>
       </c>
-      <c r="J557" t="str">
-        <v>الفصل الثاني 2024-2025</v>
-      </c>
-      <c r="K557" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="558" xml:space="preserve">
-      <c r="A558" t="str">
-        <v>مايلي صحيح عن الثاليل الشائعة ما عدا:</v>
-      </c>
-      <c r="B558" t="str">
-        <v>أشيع عند الأطفال</v>
-      </c>
-      <c r="C558" t="str">
-        <v>تتظاهر بحطاطة ذات سطح مفرط التقرن</v>
-      </c>
-      <c r="D558" t="str">
-        <v>قد تكون مفردة أو عديدة</v>
-      </c>
-      <c r="E558" t="str">
-        <v>تترافق مع حكة</v>
-      </c>
-      <c r="F558" t="str">
-        <v>تتوضع على اليدين غالباً أو قد تتوضع في أي مكان بما فيها جوف الفم</v>
-      </c>
-      <c r="G558" t="str">
-        <v>4</v>
-      </c>
-      <c r="H558" t="str" xml:space="preserve">
+      <c r="J556" t="str">
+        <v>الفصل الثاني 2024-2025</v>
+      </c>
+      <c r="K556" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="557" xml:space="preserve">
+      <c r="A557" t="str">
+        <v>أي مما يلي صحيح عن الحماق</v>
+      </c>
+      <c r="B557" t="str">
+        <v>الإصابة غير عرضية</v>
+      </c>
+      <c r="C557" t="str">
+        <v>يصيب البالغين عادة</v>
+      </c>
+      <c r="D557" t="str">
+        <v>يبقى الفيروس كامناً في الجسم بعد الإصابة</v>
+      </c>
+      <c r="E557" t="str">
+        <v>ليس له أية اختلاطات</v>
+      </c>
+      <c r="F557" t="str">
+        <v>الإصابة مؤلمة</v>
+      </c>
+      <c r="G557" t="str">
+        <v>5</v>
+      </c>
+      <c r="H557" t="str" xml:space="preserve">
         <v xml:space="preserve">
 · المرض يكون عرضياً بوضوح.
 · يصيب الأطفال بشكل رئيسي.
 · قد يؤدي إلى مضاعفات في بعض الحالات.
 · العرض الرئيسي هو حكة جلدية شديدة.</v>
       </c>
+      <c r="I557" t="str">
+        <v>جلدية</v>
+      </c>
+      <c r="J557" t="str">
+        <v>الفصل الثاني 2024-2025</v>
+      </c>
+      <c r="K557" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="str">
+        <v>مايلي صحيح عن الثاليل الشائعة ما عدا:</v>
+      </c>
+      <c r="B558" t="str">
+        <v>أشيع عند الأطفال</v>
+      </c>
+      <c r="C558" t="str">
+        <v>تتظاهر بحطاطة ذات سطح مفرط التقرن</v>
+      </c>
+      <c r="D558" t="str">
+        <v>قد تكون مفردة أو عديدة</v>
+      </c>
+      <c r="E558" t="str">
+        <v>تترافق مع حكة</v>
+      </c>
+      <c r="F558" t="str">
+        <v>تتوضع على اليدين غالباً أو قد تتوضع في أي مكان بما فيها جوف الفم</v>
+      </c>
+      <c r="G558" t="str">
+        <v>4</v>
+      </c>
+      <c r="H558" t="str">
+        <v>غير مؤلمة،غير حاكة</v>
+      </c>
       <c r="I558" t="str">
         <v>جلدية</v>
       </c>
@@ -19983,7 +19983,7 @@
         <v/>
       </c>
     </row>
-    <row r="559">
+    <row r="559" xml:space="preserve">
       <c r="A559" t="str">
         <v>مايلي صحيح عن الثاليل المسطحة ماعدا:</v>
       </c>
@@ -20005,8 +20005,11 @@
       <c r="G559" t="str">
         <v>5</v>
       </c>
-      <c r="H559" t="str">
-        <v/>
+      <c r="H559" t="str" xml:space="preserve">
+        <v xml:space="preserve">نعم، ظاهرة كوبنر موجودة في الثآليل المسطحة.
+الشرح المبسط:
+· ما هي ظاهرة كوبنر: ظهور آفات مرضية جلدية جديدة في مواقع تعرض الجلد لإصابة أو رض (مثل الخدش، الحك، الجرح).
+· في الثآليل المسطحة: عند حك أو خدش المنطقة المصابة، يمكن أن ينتشر فيروس الورم الحليمي البشري (المسبب للثاليل) إلى الجلد المجروح، مما يؤدي إلى ظهور ثاليل مسطحة جديدة في خطوط أو مسار الإصابة.</v>
       </c>
       <c r="I559" t="str">
         <v>جلدية</v>
@@ -20041,7 +20044,7 @@
         <v>2</v>
       </c>
       <c r="H560" t="str">
-        <v/>
+        <v>يبدا في الثنايا العميقة وينتشر</v>
       </c>
       <c r="I560" t="str">
         <v>جلدية</v>
@@ -20076,7 +20079,7 @@
         <v>3</v>
       </c>
       <c r="H561" t="str">
-        <v/>
+        <v>كتلة تشبه القرنبيط</v>
       </c>
       <c r="I561" t="str">
         <v>جلدية</v>
@@ -20111,7 +20114,7 @@
         <v>2</v>
       </c>
       <c r="H562" t="str">
-        <v/>
+        <v>وسوف بيضاء عالجذع والاطراف مميزة</v>
       </c>
       <c r="I562" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 2:27:11 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -20254,7 +20254,7 @@
         <v>3</v>
       </c>
       <c r="H566" t="str">
-        <v/>
+        <v>حكة خفيفة احيانا</v>
       </c>
       <c r="I566" t="str">
         <v>جلدية</v>
@@ -20289,7 +20289,7 @@
         <v>5</v>
       </c>
       <c r="H567" t="str">
-        <v/>
+        <v xml:space="preserve">حاصة غير ندبية </v>
       </c>
       <c r="I567" t="str">
         <v>جلدية</v>
@@ -20324,7 +20324,7 @@
         <v>3</v>
       </c>
       <c r="H568" t="str">
-        <v/>
+        <v>حاصة غير ندبية</v>
       </c>
       <c r="I568" t="str">
         <v>جلدية</v>
@@ -20359,7 +20359,7 @@
         <v>3</v>
       </c>
       <c r="H569" t="str">
-        <v/>
+        <v>يحصل تشنج وعائي حاد يليه التهاب</v>
       </c>
       <c r="I569" t="str">
         <v>جلدية</v>
@@ -20394,7 +20394,7 @@
         <v>3</v>
       </c>
       <c r="H570" t="str">
-        <v/>
+        <v>مفرط الجفاف</v>
       </c>
       <c r="I570" t="str">
         <v>جلدية</v>
@@ -20429,7 +20429,7 @@
         <v>2</v>
       </c>
       <c r="H571" t="str">
-        <v/>
+        <v>تنمو ببطء ولا تتراجع عفويا</v>
       </c>
       <c r="I571" t="str">
         <v>جلدية</v>
@@ -20464,7 +20464,7 @@
         <v>4</v>
       </c>
       <c r="H572" t="str">
-        <v/>
+        <v>ندبات دائمة</v>
       </c>
       <c r="I572" t="str">
         <v>جلدية</v>
@@ -20499,7 +20499,7 @@
         <v>2</v>
       </c>
       <c r="H573" t="str">
-        <v/>
+        <v>قد يحدث كمضاعفة وليس تظاهر سريري</v>
       </c>
       <c r="I573" t="str">
         <v>جلدية</v>
@@ -20511,7 +20511,7 @@
         <v/>
       </c>
     </row>
-    <row r="574">
+    <row r="574" xml:space="preserve">
       <c r="A574" t="str">
         <v>ما يلي صحيح عن الليشمانيا ما عدا:</v>
       </c>
@@ -20533,8 +20533,10 @@
       <c r="G574" t="str">
         <v>1</v>
       </c>
-      <c r="H574" t="str">
-        <v/>
+      <c r="H574" t="str" xml:space="preserve">
+        <v xml:space="preserve">فترة الحضانة: أسبوعين إلى عدة أشهر.
+فترة النمو: أسابيع إلى أشهر.
+فترة التراجع: 6 أشهر إلى سنة أو أكثر.</v>
       </c>
       <c r="I574" t="str">
         <v>جلدية</v>
@@ -20546,7 +20548,7 @@
         <v/>
       </c>
     </row>
-    <row r="575">
+    <row r="575" xml:space="preserve">
       <c r="A575" t="str">
         <v>ما يلي من أنماط الإكزيمة داخلية المنشأ ما عدا:</v>
       </c>
@@ -20568,8 +20570,15 @@
       <c r="G575" t="str">
         <v>4</v>
       </c>
-      <c r="H575" t="str">
-        <v/>
+      <c r="H575" t="str" xml:space="preserve">
+        <v xml:space="preserve">أنواع الإكزيما ذات المنشأ الداخلي (غير التحسسية للتماس في الغالب):
+1. الإكزيما التأتبية (Atopic eczema)
+2. إكزيما الدوالي (Varicose eczema)
+3. الإكزيما الدهنية (Seborrhoeic eczema)
+4. إكزيما عسر التعرق (Pompholyx/Dyshidrotic eczema)
+5. الإكزيما القرصية (Nummular eczema)
+6. إكزيما الحلمات (في غير المرضع)
+7. إكزيما اليدين والقدمين (الأنواع غير المرتبطة بالتماس المباشر)</v>
       </c>
       <c r="I575" t="str">
         <v>جلدية</v>
@@ -20581,7 +20590,7 @@
         <v/>
       </c>
     </row>
-    <row r="576">
+    <row r="576" xml:space="preserve">
       <c r="A576" t="str">
         <v>ما يلي صحيح عن قمال الجسد:</v>
       </c>
@@ -20603,8 +20612,12 @@
       <c r="G576" t="str">
         <v>5</v>
       </c>
-      <c r="H576" t="str">
-        <v/>
+      <c r="H576" t="str" xml:space="preserve">
+        <v xml:space="preserve">التصحيح:
+1. سبب الحكة: رد فعل تحسسي للعاب وبراز الطفيلي.
+2. المرض: مزمن.
+3. العرض الرئيسي: الحكة الشديدة.
+4. طريقة التغذية: بامتصاص الدم.</v>
       </c>
       <c r="I576" t="str">
         <v>جلدية</v>
@@ -20639,7 +20652,7 @@
         <v>4</v>
       </c>
       <c r="H577" t="str">
-        <v/>
+        <v>لا يستطيع اختراق الطبقة القرنية السميكة فيها</v>
       </c>
       <c r="I577" t="str">
         <v>جلدية</v>
@@ -20674,7 +20687,7 @@
         <v>3</v>
       </c>
       <c r="H578" t="str">
-        <v/>
+        <v>الانتبارات</v>
       </c>
       <c r="I578" t="str">
         <v>جلدية</v>
@@ -20709,7 +20722,7 @@
         <v>3</v>
       </c>
       <c r="H579" t="str">
-        <v/>
+        <v>شائع جدا ومميز للمرض</v>
       </c>
       <c r="I579" t="str">
         <v>جلدية</v>
@@ -20744,7 +20757,7 @@
         <v>5</v>
       </c>
       <c r="H580" t="str">
-        <v/>
+        <v>HSV1,2</v>
       </c>
       <c r="I580" t="str">
         <v>جلدية</v>
@@ -20756,7 +20769,7 @@
         <v/>
       </c>
     </row>
-    <row r="581">
+    <row r="581" xml:space="preserve">
       <c r="A581" t="str">
         <v>ما يلي صحيح عن تنخر البشرة السمي ماعدا:</v>
       </c>
@@ -20778,8 +20791,9 @@
       <c r="G581" t="str">
         <v>4</v>
       </c>
-      <c r="H581" t="str">
-        <v/>
+      <c r="H581" t="str" xml:space="preserve">
+        <v xml:space="preserve">الدوائي 90%
+الانتاني لا يتعدى 5%</v>
       </c>
       <c r="I581" t="str">
         <v>جلدية</v>
@@ -20814,7 +20828,7 @@
         <v>2</v>
       </c>
       <c r="H582" t="str">
-        <v/>
+        <v>فروة،وسط الوجه، صدر وظهر وثنيات</v>
       </c>
       <c r="I582" t="str">
         <v>جلدية</v>
@@ -20849,7 +20863,7 @@
         <v>5</v>
       </c>
       <c r="H583" t="str">
-        <v/>
+        <v>رقيق، ناعم،هش</v>
       </c>
       <c r="I583" t="str">
         <v>جلدية</v>
@@ -20884,7 +20898,7 @@
         <v>3</v>
       </c>
       <c r="H584" t="str">
-        <v/>
+        <v>انسداد الجريبة الشعرية) المسام(</v>
       </c>
       <c r="I584" t="str">
         <v>جلدية</v>
@@ -20919,7 +20933,7 @@
         <v>5</v>
       </c>
       <c r="H585" t="str">
-        <v/>
+        <v>اصابة الفروة ندبية</v>
       </c>
       <c r="I585" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 2:36:15 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -21015,7 +21015,7 @@
         <v/>
       </c>
     </row>
-    <row r="588">
+    <row r="588" xml:space="preserve">
       <c r="A588" t="str">
         <v>أي العبارات التالية عن أشعة الليزر خاطئة:</v>
       </c>
@@ -21037,8 +21037,11 @@
       <c r="G588" t="str">
         <v>3</v>
       </c>
-      <c r="H588" t="str">
-        <v>-</v>
+      <c r="H588" t="str" xml:space="preserve">
+        <v xml:space="preserve">الاحمرة الجلدية(Erythroderma) هي حالة جلدية مهددة للحياة يتميز فيها أكثر من 90% من سطح الجسم بالاحمرار والتهاب وتقشّر شديد، وغالباً ما تكون مضاعفة لمرض جلدي أو دوائي أو جهازي موجود مسبقاً.
+1. الليزر يضر ولا ينفع: الجلد ملتهب ورقيق، والليزر سيسبب حروقاً وتقرحات.
+2. ليس حلاً جذرياً: الاحمرار عرض لمرض آخر (صداف، إكزيما)، والعلاج يكون بمعالجة السبب الأساسي، وليس بحرق السطح.
+3. خطر على الحياة: حالة المريض العامة حرجة، والليزر إجراء تجميلي غير آمن في هذه الحالة الطارئة.</v>
       </c>
       <c r="I588" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 2:45:55 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -21193,7 +21193,7 @@
         <v/>
       </c>
     </row>
-    <row r="593">
+    <row r="593" xml:space="preserve">
       <c r="A593" t="str">
         <v>من التظاهرات الجلدية لأمراض الكبد ماعدا:</v>
       </c>
@@ -21215,8 +21215,12 @@
       <c r="G593" t="str">
         <v>4</v>
       </c>
-      <c r="H593" t="str">
-        <v/>
+      <c r="H593" t="str" xml:space="preserve">
+        <v xml:space="preserve">اليرقان (اصفرار الجلد)
+· الحكة
+· الأورمة الوعائية العنكبوتية
+· احمرار راحتي اليدين
+· دوالي الساقين</v>
       </c>
       <c r="I593" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 2:47:44 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -21232,7 +21232,7 @@
         <v/>
       </c>
     </row>
-    <row r="594">
+    <row r="594" xml:space="preserve">
       <c r="A594" t="str">
         <v>أي العبارات التالية عن غرن كابوزي صحيحة:</v>
       </c>
@@ -21254,8 +21254,11 @@
       <c r="G594" t="str">
         <v>4</v>
       </c>
-      <c r="H594" t="str">
-        <v/>
+      <c r="H594" t="str" xml:space="preserve">
+        <v xml:space="preserve">يصيب الأغشية المخاطية (خاصة الفم).
+   · قد يصيب الأعضاء الداخلية (مثل القناة الهضمية والرئتين).
+   · يصيب الشكل الكلاسيكي كبار السن من أصل متوسطي أو شرق أوروبي.
+   · ورم وعائي ينشأ من الخلايا البطانية للأوعية الدموية أو اللمفاوية.</v>
       </c>
       <c r="I594" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 3:09:22 AM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -21402,7 +21402,7 @@
         <v/>
       </c>
     </row>
-    <row r="601" xml:space="preserve">
+    <row r="601">
       <c r="A601" t="str">
         <v>ما يلي صحيح عن صلابة الجلد الجهازية ماعدا:</v>
       </c>
@@ -21424,9 +21424,8 @@
       <c r="G601" t="str">
         <v>2</v>
       </c>
-      <c r="H601" t="str" xml:space="preserve">
-        <v xml:space="preserve">Anti-Centromere Antibodies 70%
-Scl-70 (30-40%)</v>
+      <c r="H601" t="str">
+        <v>Anti-Centromere Antibodies 70%Scl-70 (30-40%)</v>
       </c>
       <c r="I601" t="str">
         <v>جلدية</v>
@@ -21496,7 +21495,7 @@
         <v>3</v>
       </c>
       <c r="H603" t="str">
-        <v/>
+        <v>3 اسابيع</v>
       </c>
       <c r="I603" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 12:37:36 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -20022,10 +20022,10 @@
         <v>ينمو بسرعة</v>
       </c>
       <c r="G561" t="str">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H561" t="str">
-        <v>كتلة تشبه القرنبيط</v>
+        <v>يستمر في النمو والانتشار موضعيا وتدمير الانسجة حوله</v>
       </c>
       <c r="I561" t="str">
         <v>جلدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 12:45:00 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -7682,7 +7682,7 @@
         <v/>
       </c>
     </row>
-    <row r="209">
+    <row r="209" xml:space="preserve">
       <c r="A209" t="str">
         <v>سرطان الغدة الكظرية</v>
       </c>
@@ -7702,10 +7702,12 @@
         <v>اعمار متقدمة</v>
       </c>
       <c r="G209" t="str">
-        <v>5</v>
-      </c>
-      <c r="H209" t="str">
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="H209" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+سنين الاصابة هيه بين ٥٠ و ٦٠
+او الاطفال</v>
       </c>
       <c r="I209" t="str">
         <v>داخلية غدية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 1:05:55 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -7682,7 +7682,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" xml:space="preserve">
+    <row r="209">
       <c r="A209" t="str">
         <v>سرطان الغدة الكظرية</v>
       </c>
@@ -7704,10 +7704,8 @@
       <c r="G209" t="str">
         <v>4</v>
       </c>
-      <c r="H209" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-سنين الاصابة هيه بين ٥٠ و ٦٠
-او الاطفال</v>
+      <c r="H209" t="str">
+        <v>سنين الاصابة هيه بين ٥٠ و ٦٠او الاطفال</v>
       </c>
       <c r="I209" t="str">
         <v>داخلية غدية</v>
@@ -7716,7 +7714,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K209" t="str">
-        <v/>
+        <v>تصويبات</v>
       </c>
     </row>
     <row r="210">
@@ -20036,7 +20034,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K561" t="str">
-        <v/>
+        <v>تصويبات</v>
       </c>
     </row>
     <row r="562">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 2:15:53 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -16032,10 +16032,10 @@
         <v/>
       </c>
       <c r="G447" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H447" t="str">
-        <v/>
+        <v>هون كلن صح عمليا بس الاقرب للخطأ هي b</v>
       </c>
       <c r="I447" t="str">
         <v>داخلية رثوية</v>
@@ -16044,7 +16044,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K447" t="str">
-        <v/>
+        <v>تصويبات</v>
       </c>
     </row>
     <row r="448">
@@ -17727,7 +17727,7 @@
         <v/>
       </c>
     </row>
-    <row r="496">
+    <row r="496" xml:space="preserve">
       <c r="A496" t="str">
         <v>الخاطئة عن التهاب المفاصل الصدافي</v>
       </c>
@@ -17747,10 +17747,11 @@
         <v/>
       </c>
       <c r="G496" t="str">
-        <v>4</v>
-      </c>
-      <c r="H496" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="H496" t="str" xml:space="preserve">
+        <v xml:space="preserve">A يسبب تاكلات فقط
+B ١٠-١٥٪ المفصل قبل الجلد بتتحمل تكون غلط</v>
       </c>
       <c r="I496" t="str">
         <v>داخلية رثوية</v>
@@ -17759,7 +17760,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K496" t="str">
-        <v/>
+        <v>تصويبات</v>
       </c>
     </row>
     <row r="497">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 9/30/2025, 10:36:28 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -17727,7 +17727,7 @@
         <v/>
       </c>
     </row>
-    <row r="496" xml:space="preserve">
+    <row r="496">
       <c r="A496" t="str">
         <v>الخاطئة عن التهاب المفاصل الصدافي</v>
       </c>
@@ -17747,11 +17747,10 @@
         <v/>
       </c>
       <c r="G496" t="str">
-        <v>1</v>
-      </c>
-      <c r="H496" t="str" xml:space="preserve">
-        <v xml:space="preserve">A يسبب تاكلات فقط
-B ١٠-١٥٪ المفصل قبل الجلد بتتحمل تكون غلط</v>
+        <v>4</v>
+      </c>
+      <c r="H496" t="str">
+        <v/>
       </c>
       <c r="I496" t="str">
         <v>داخلية رثوية</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 02:53:05
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -1207,9 +1207,9 @@
         <v>النزف</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" xml:space="preserve">
       <c r="A24" t="str">
-        <v>في تقييم النزف الهضمي العلوي الحاد، تم تركيب NGT وكانت الرشافة رائقة، نستنتج: ( اختر الصحيحة ) (قارن مع سؤال جراحة 1 دورة 2024  2025، الفصل الأول  السؤال رقم 62 )</v>
+        <v xml:space="preserve">في تقييم النزف الهضمي العلوي الحاد، تم تركيب NGT وكانت الرشافة رائقة، نستنتج: ( اختر الصحيحة ) </v>
       </c>
       <c r="B24" t="str">
         <v>موقع النزف بعد البواب حتماً</v>
@@ -1221,7 +1221,7 @@
         <v>يعتبر الكولون مصدر النزف</v>
       </c>
       <c r="E24" t="str">
-        <v>نفي النزف الهضمي العلوي ✅</v>
+        <v xml:space="preserve">نفي النزف الهضمي العلوي </v>
       </c>
       <c r="F24" t="str">
         <v/>
@@ -1229,8 +1229,9 @@
       <c r="G24" t="str">
         <v>2</v>
       </c>
-      <c r="H24" t="str">
-        <v/>
+      <c r="H24" t="str" xml:space="preserve">
+        <v xml:space="preserve">(قارن مع سؤال جراحة 1 دورة 2024  2025، الفصل الأول  السؤال رقم 62 ) ...
+السؤال ببيتا نفس هاد تماما ونفس الحل بس هنيك مكتوب اختر الخطا</v>
       </c>
       <c r="I24" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 03:12:22
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -1651,7 +1651,7 @@
         <v>2</v>
       </c>
       <c r="H36" t="str">
-        <v/>
+        <v>الحالات المختلطة بانثقاب يصبح الالم معمم وقد يبقى موضعي</v>
       </c>
       <c r="I36" t="str">
         <v>جراحة 1</v>
@@ -1663,12 +1663,12 @@
         <v>زائدة</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" xml:space="preserve">
       <c r="A37" t="str">
-        <v>في أورام الزائدة الدودية ماعدا: B أو D</v>
+        <v xml:space="preserve">في أورام الزائدة الدودية ماعدا: </v>
       </c>
       <c r="B37" t="str">
-        <v>تعتبر الزائدة الدودية اهم توضع لبورم السرطاوي</v>
+        <v>تعتبر الزائدة الدودية اهم توضع للورم السرطاوي</v>
       </c>
       <c r="C37" t="str">
         <v>قد تترافق القيلة المخاطية مع الحبن الهلامي</v>
@@ -1683,10 +1683,11 @@
         <v/>
       </c>
       <c r="G37" t="str">
-        <v>4</v>
-      </c>
-      <c r="H37" t="str">
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="H37" t="str" xml:space="preserve">
+        <v xml:space="preserve"> تترافق القيلة المخاطية في حالات قليلة مع حدوث الحبن الهلامي
+والمعروف أيضا باسم المخاطوم الكاذب </v>
       </c>
       <c r="I37" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 13:23:16
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -670,7 +670,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="str">
-        <v/>
+        <v>التفسير يستخدم في الاحلات الاسعافية  للكشف عن وجود دم حر في البطن</v>
       </c>
       <c r="I8" t="str">
         <v>جراحة 1</v>
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="H13" t="str">
-        <v/>
+        <v>فانيليل ماندليك اسيد هو من نتائج استقلاب الادرينالين و نور ادرينالين</v>
       </c>
       <c r="I13" t="str">
         <v>جراحة 1</v>
@@ -892,7 +892,7 @@
         <v>كظر</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" xml:space="preserve">
       <c r="A15" t="str">
         <v>‏يعالج الشق الشرجي بما يلي عدا</v>
       </c>
@@ -914,8 +914,9 @@
       <c r="G15" t="str">
         <v>4</v>
       </c>
-      <c r="H15" t="str">
-        <v/>
+      <c r="H15" t="str" xml:space="preserve">
+        <v xml:space="preserve"> خزع الداخلية وليس الخارجية
+الهارجية تؤدي الى سلس</v>
       </c>
       <c r="I15" t="str">
         <v>جراحة 1</v>
@@ -1055,7 +1056,7 @@
         <v>2</v>
       </c>
       <c r="H19" t="str">
-        <v/>
+        <v>بشكل متقطع وليس مستمر</v>
       </c>
       <c r="I19" t="str">
         <v>جراحة 1</v>
@@ -1207,7 +1208,7 @@
         <v>النزف</v>
       </c>
     </row>
-    <row r="24" xml:space="preserve">
+    <row r="24">
       <c r="A24" t="str">
         <v xml:space="preserve">في تقييم النزف الهضمي العلوي الحاد، تم تركيب NGT وكانت الرشافة رائقة، نستنتج: ( اختر الصحيحة ) </v>
       </c>
@@ -1229,9 +1230,8 @@
       <c r="G24" t="str">
         <v>2</v>
       </c>
-      <c r="H24" t="str" xml:space="preserve">
-        <v xml:space="preserve">(قارن مع سؤال جراحة 1 دورة 2024  2025، الفصل الأول  السؤال رقم 62 ) ...
-السؤال ببيتا نفس هاد تماما ونفس الحل بس هنيك مكتوب اختر الخطا</v>
+      <c r="H24" t="str">
+        <v>(قارن مع سؤال جراحة 1 دورة 2024  2025، الفصل الأول  السؤال رقم 62 ) ...السؤال ببيتا نفس هاد تماما ونفس الحل بس هنيك مكتوب اختر الخطا</v>
       </c>
       <c r="I24" t="str">
         <v>جراحة 1</v>
@@ -1476,7 +1476,7 @@
         <v>4</v>
       </c>
       <c r="H31" t="str">
-        <v/>
+        <v>ماعدا</v>
       </c>
       <c r="I31" t="str">
         <v>جراحة 1</v>
@@ -1511,7 +1511,7 @@
         <v>3</v>
       </c>
       <c r="H32" t="str">
-        <v/>
+        <v>السل العلاج دوائي</v>
       </c>
       <c r="I32" t="str">
         <v>جراحة 1</v>
@@ -1543,10 +1543,10 @@
         <v xml:space="preserve">يختلط أحيانا نزف معوي غزير أو انغلاف معوي </v>
       </c>
       <c r="G33" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H33" t="str">
-        <v/>
+        <v>فرصة التحول للخباثة قريب ٣%</v>
       </c>
       <c r="I33" t="str">
         <v>جراحة 1</v>
@@ -1663,7 +1663,7 @@
         <v>زائدة</v>
       </c>
     </row>
-    <row r="37" xml:space="preserve">
+    <row r="37">
       <c r="A37" t="str">
         <v xml:space="preserve">في أورام الزائدة الدودية ماعدا: </v>
       </c>
@@ -1685,9 +1685,8 @@
       <c r="G37" t="str">
         <v>3</v>
       </c>
-      <c r="H37" t="str" xml:space="preserve">
-        <v xml:space="preserve"> تترافق القيلة المخاطية في حالات قليلة مع حدوث الحبن الهلامي
-والمعروف أيضا باسم المخاطوم الكاذب </v>
+      <c r="H37" t="str">
+        <v xml:space="preserve"> تترافق القيلة المخاطية في حالات قليلة مع حدوث الحبن الهلاميوالمعروف أيضا باسم المخاطوم الكاذب </v>
       </c>
       <c r="I37" t="str">
         <v>جراحة 1</v>
@@ -1789,7 +1788,7 @@
         <v>الجراحة هي الحل الأمثل للعلاج</v>
       </c>
       <c r="G40" t="str">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H40" t="str">
         <v/>
@@ -1827,7 +1826,7 @@
         <v>2</v>
       </c>
       <c r="H41" t="str">
-        <v/>
+        <v>قلاء استقلابي</v>
       </c>
       <c r="I41" t="str">
         <v>جراحة 1</v>
@@ -1859,10 +1858,10 @@
         <v xml:space="preserve">يستجيب للعلاج الشعاعي اكثر من الكيماوي </v>
       </c>
       <c r="G42" t="str">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H42" t="str">
-        <v/>
+        <v>الاشيع في علاجات سرطان جاهز الهضم هو الكيميائي (يحتاج تاكد)</v>
       </c>
       <c r="I42" t="str">
         <v>جراحة 1</v>
@@ -1932,7 +1931,7 @@
         <v>2</v>
       </c>
       <c r="H44" t="str">
-        <v/>
+        <v>كوشينغ اسمها</v>
       </c>
       <c r="I44" t="str">
         <v>جراحة 1</v>
@@ -2212,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="H52" t="str">
-        <v/>
+        <v xml:space="preserve"> انسداد الامعاء العرض الاشيع بالكولون الايسر</v>
       </c>
       <c r="I52" t="str">
         <v>جراحة 1</v>
@@ -2247,7 +2246,7 @@
         <v>3</v>
       </c>
       <c r="H53" t="str">
-        <v/>
+        <v>يحتاج تدقيق من المقرر</v>
       </c>
       <c r="I53" t="str">
         <v>جراحة 1</v>
@@ -2574,7 +2573,7 @@
         <v>قولون</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" xml:space="preserve">
       <c r="A63" t="str">
         <v>في تدبير انفتال السين المتموت كل مايلي صحيح عدا:</v>
       </c>
@@ -2594,10 +2593,13 @@
         <v/>
       </c>
       <c r="G63" t="str">
-        <v>1</v>
-      </c>
-      <c r="H63" t="str">
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="H63" t="str" xml:space="preserve">
+        <v xml:space="preserve">العلاج بالأنبوب المستقيمي ❌  
+  صحيح فقط في الانفتال غير المتموت (كوسيلة مؤقتة لفك الانفتال بالمنظار أو الأنبوب).  
+  في حال وجود تموت أو غرغرينا، لا يجوز الاعتماد على هذه الطريقة، ويجب التدخل الجراحي الفوري.
+</v>
       </c>
       <c r="I63" t="str">
         <v>جراحة 1</v>
@@ -2629,10 +2631,10 @@
         <v/>
       </c>
       <c r="G64" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H64" t="str">
-        <v/>
+        <v>يحتاج تدقيق</v>
       </c>
       <c r="I64" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 13:46:23
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -1135,7 +1135,7 @@
         <v>الفصل الثاني 20242025</v>
       </c>
       <c r="K21" t="str">
-        <v>النزف</v>
+        <v>جدار البطن</v>
       </c>
     </row>
     <row r="22">
@@ -1975,7 +1975,7 @@
         <v>الفصل الثاني 20242025</v>
       </c>
       <c r="K45" t="str">
-        <v>الأمعاء</v>
+        <v>جدار البطن</v>
       </c>
     </row>
     <row r="46">
@@ -2080,7 +2080,7 @@
         <v>الفصل الثاني 20242025</v>
       </c>
       <c r="K48" t="str">
-        <v>الأمعاء</v>
+        <v>جدار البطن</v>
       </c>
     </row>
     <row r="49">
@@ -2115,7 +2115,7 @@
         <v>الفصل الثاني 20242025</v>
       </c>
       <c r="K49" t="str">
-        <v>الأمعاء</v>
+        <v>جدار البطن</v>
       </c>
     </row>
     <row r="50">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 14:24:06
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -2488,10 +2488,10 @@
         <v/>
       </c>
       <c r="G60" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H60" t="str">
-        <v/>
+        <v>قارن مع 41 دورة 2024-2025 فصل أول</v>
       </c>
       <c r="I60" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 16:04:50
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -892,7 +892,7 @@
         <v>كظر</v>
       </c>
     </row>
-    <row r="15" xml:space="preserve">
+    <row r="15">
       <c r="A15" t="str">
         <v>‏يعالج الشق الشرجي بما يلي عدا</v>
       </c>
@@ -914,9 +914,8 @@
       <c r="G15" t="str">
         <v>4</v>
       </c>
-      <c r="H15" t="str" xml:space="preserve">
-        <v xml:space="preserve"> خزع الداخلية وليس الخارجية
-الهارجية تؤدي الى سلس</v>
+      <c r="H15" t="str">
+        <v xml:space="preserve"> خزع الداخلية وليس الخارجيةالهارجية تؤدي الى سلس</v>
       </c>
       <c r="I15" t="str">
         <v>جراحة 1</v>
@@ -2573,7 +2572,7 @@
         <v>قولون</v>
       </c>
     </row>
-    <row r="63" xml:space="preserve">
+    <row r="63">
       <c r="A63" t="str">
         <v>في تدبير انفتال السين المتموت كل مايلي صحيح عدا:</v>
       </c>
@@ -2595,11 +2594,8 @@
       <c r="G63" t="str">
         <v>2</v>
       </c>
-      <c r="H63" t="str" xml:space="preserve">
-        <v xml:space="preserve">العلاج بالأنبوب المستقيمي ❌  
-  صحيح فقط في الانفتال غير المتموت (كوسيلة مؤقتة لفك الانفتال بالمنظار أو الأنبوب).  
-  في حال وجود تموت أو غرغرينا، لا يجوز الاعتماد على هذه الطريقة، ويجب التدخل الجراحي الفوري.
-</v>
+      <c r="H63" t="str">
+        <v>العلاج بالأنبوب المستقيمي ❌    صحيح فقط في الانفتال غير المتموت (كوسيلة مؤقتة لفك الانفتال بالمنظار أو الأنبوب).    في حال وجود تموت أو غرغرينا، لا يجوز الاعتماد على هذه الطريقة، ويجب التدخل الجراحي الفوري.</v>
       </c>
       <c r="I63" t="str">
         <v>جراحة 1</v>
@@ -8651,10 +8647,10 @@
         <v>ذات عظم ونقي حاد بعظم العقب</v>
       </c>
       <c r="G236" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H236" t="str">
-        <v/>
+        <v>بقية الخيارات منعمل بتر ساق مو بتر قدم</v>
       </c>
       <c r="I236" t="str">
         <v>جراحة 4</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 02/10/2025, 19:40:06
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -2475,7 +2475,7 @@
         <v>يعد الالم البطني عرضا لا نوعيا لكل قسم من اقسام الكولون</v>
       </c>
       <c r="C60" t="str">
-        <v>النزف الدموي الضهمي الزفتي هو دائما كولوني المنشأ</v>
+        <v>النزف الدموي الهضمي الزفتي هو دائما كولوني المنشأ</v>
       </c>
       <c r="D60" t="str">
         <v>يتظاهر  انسداد الامعاء كولوني المنشأ بإمساك باكر</v>
@@ -2487,10 +2487,10 @@
         <v/>
       </c>
       <c r="G60" t="str">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H60" t="str">
-        <v>قارن مع 41 دورة 2024-2025 فصل أول</v>
+        <v xml:space="preserve">قارن مع 41 دورة 2024-2025 فصل أول... بهاسؤال اخترنا الغلط لان النزف العلوي بكون زفتي </v>
       </c>
       <c r="I60" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 03/10/2025, 01:01:23
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -1157,10 +1157,10 @@
         <v/>
       </c>
       <c r="G22" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22" t="str">
-        <v>هاد لازم يكون اختر الخطأ ... (غالبا مخربطين بتجميعه موجود نفسه بالحرف ببيتا بنفس الحل بس هنيك مكتوب اختر الخطأ)</v>
+        <v/>
       </c>
       <c r="I22" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 03/10/2025, 11:24:08
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -2242,7 +2242,7 @@
         <v/>
       </c>
       <c r="G53" t="str">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H53" t="str">
         <v>يحتاج تدقيق من المقرر</v>
@@ -2642,7 +2642,7 @@
         <v>الأمعاء</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" xml:space="preserve">
       <c r="A65" t="str">
         <v>في تشوه ايبشتاين كل ما يلي صحيح ما عدا:</v>
       </c>
@@ -2664,8 +2664,12 @@
       <c r="G65" t="str">
         <v>1</v>
       </c>
-      <c r="H65" t="str">
-        <v/>
+      <c r="H65" t="str" xml:space="preserve">
+        <v xml:space="preserve">يصيب فقط الطرف الايمن
+بصير عندي توسع للاذينة اليمنى على حساب البطين الايمن
+التاجي مالوش دعوة
+بسبب انو توضع ثلاثي الشرف بجي منخفض
+</v>
       </c>
       <c r="I65" t="str">
         <v>جراحة 2</v>
@@ -2805,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="str">
-        <v/>
+        <v>الابهري اشيع</v>
       </c>
       <c r="I69" t="str">
         <v>جراحة 2</v>
@@ -2840,7 +2844,7 @@
         <v>4</v>
       </c>
       <c r="H70" t="str">
-        <v/>
+        <v>لا يتوسع انما يتضخم</v>
       </c>
       <c r="I70" t="str">
         <v>جراحة 2</v>
@@ -2992,7 +2996,7 @@
         <v>قلبية</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" xml:space="preserve">
       <c r="A75" t="str">
         <v>في الصمام التاجي كل ما يلي صحيح عدا:</v>
       </c>
@@ -3014,8 +3018,9 @@
       <c r="G75" t="str">
         <v>3</v>
       </c>
-      <c r="H75" t="str">
-        <v/>
+      <c r="H75" t="str" xml:space="preserve">
+        <v xml:space="preserve"> تتمزق هذه الحليمة بالاحتشاء بسبب ترويتها بشريان وحيد
+</v>
       </c>
       <c r="I75" t="str">
         <v>جراحة 2</v>
@@ -4112,7 +4117,7 @@
         <v>قلبية</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" xml:space="preserve">
       <c r="A107" t="str">
         <v>من مضادات استطباب زرع القلب كل ما يلي صحيح عدا:</v>
       </c>
@@ -4134,8 +4139,9 @@
       <c r="G107" t="str">
         <v>4</v>
       </c>
-      <c r="H107" t="str">
-        <v/>
+      <c r="H107" t="str" xml:space="preserve">
+        <v xml:space="preserve">التفسير هو حدوث استجابة التهابية شديدة
+تؤدي الى تخثر منتشر في الاوعية و ليس فرط نمو بطانة</v>
       </c>
       <c r="I107" t="str">
         <v>جراحة 2</v>
@@ -4205,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="H109" t="str">
-        <v/>
+        <v>الورم المذكور سليم</v>
       </c>
       <c r="I109" t="str">
         <v>جراحة 2</v>
@@ -4310,7 +4316,7 @@
         <v>3</v>
       </c>
       <c r="H112" t="str">
-        <v/>
+        <v>تزيد المقاومة وليست تنقص</v>
       </c>
       <c r="I112" t="str">
         <v>جراحة 2</v>
@@ -4870,7 +4876,7 @@
         <v>4</v>
       </c>
       <c r="H128" t="str">
-        <v/>
+        <v>يحدث امتداد للعظم في المراحل المتقدمة فقط</v>
       </c>
       <c r="I128" t="str">
         <v>جراحة 2</v>
@@ -4882,7 +4888,7 @@
         <v>صدرية</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" xml:space="preserve">
       <c r="A129" t="str">
         <v>يستطب فتح الصدر الجراحي في تدمي الجنب:</v>
       </c>
@@ -4904,8 +4910,9 @@
       <c r="G129" t="str">
         <v>2</v>
       </c>
-      <c r="H129" t="str">
-        <v/>
+      <c r="H129" t="str" xml:space="preserve">
+        <v xml:space="preserve">مع استرواح الصدر يعالج بتفجير الصدر بشكل مبدئي
+اذا فشل ننتقل الى الجراحي</v>
       </c>
       <c r="I129" t="str">
         <v>جراحة 2</v>
@@ -5022,7 +5029,7 @@
         <v>صدرية</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" xml:space="preserve">
       <c r="A133" t="str">
         <v>اذيات القناة الصدريه الرضيه:</v>
       </c>
@@ -5044,8 +5051,13 @@
       <c r="G133" t="str">
         <v>4</v>
       </c>
-      <c r="H133" t="str">
-        <v/>
+      <c r="H133" t="str" xml:space="preserve">
+        <v xml:space="preserve">الخيار الاول الانصباب الكيلوسي (Chylothorax) يكون عادةً عكراً/لبنياً بسبب وجود الكيلوس (غني بالشحوم).  
+  لا يكون محجباً (loculated) منذ البداية، بل قد يصبح كذلك لاحقاً إذا استمر أو حدث التهاب ثانوي.  
+الخيار الثاني - العلاج المحافظ يعتمد على حمية قليلة الدسم (خصوصاً الدهون طويلة السلسلة) مع إعطاء دهون متوسطة السلسلة (MCT) لأنها تُمتص مباشرة إلى الدوران البابي ولا تمر بالقناة الصدرية.
+الخيار الثالث  ...  - العلاج يبدأ محافظاً (حمية + تصريف + دعم غذائي ± أوكتريوتيد).  
+  - الجراحة (ربط القناة الصدرية أو تحويلة) تُجرى فقط إذا فشل العلاج المحافظ أو كان التسريب غزيراً مستمراً.
+  - ليست الحمية الخالية من البروتين.  </v>
       </c>
       <c r="I133" t="str">
         <v>جراحة 2</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 03/10/2025, 11:33:18
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -5174,7 +5174,7 @@
         <v>صدرية</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" xml:space="preserve">
       <c r="A137" t="str">
         <v>اذية المري الرضية:</v>
       </c>
@@ -5194,10 +5194,14 @@
         <v/>
       </c>
       <c r="G137" t="str">
-        <v>1</v>
-      </c>
-      <c r="H137" t="str">
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="H137" t="str" xml:space="preserve">
+        <v xml:space="preserve">طلع بالبحث اصابته صعبة لانو محمي بالقصبات
+و ممكن انظر 
+وممكن يسبب استرواح صدر
+في اكثر من اجابة صح
+معناها الها علاقة منهاج الدكتور</v>
       </c>
       <c r="I137" t="str">
         <v>جراحة 2</v>
@@ -5232,7 +5236,7 @@
         <v>3</v>
       </c>
       <c r="H138" t="str">
-        <v/>
+        <v>غالبا السؤال ما عدا</v>
       </c>
       <c r="I138" t="str">
         <v>جراحة 2</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 03/10/2025, 14:24:18
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -1787,10 +1787,10 @@
         <v>الجراحة هي الحل الأمثل للعلاج</v>
       </c>
       <c r="G40" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H40" t="str">
-        <v/>
+        <v>اخترنا الخاطئة... جراحة المعدة اسعافية</v>
       </c>
       <c r="I40" t="str">
         <v>جراحة 1</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 04/10/2025, 11:20:07
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -2642,7 +2642,7 @@
         <v>الأمعاء</v>
       </c>
     </row>
-    <row r="65" xml:space="preserve">
+    <row r="65">
       <c r="A65" t="str">
         <v>في تشوه ايبشتاين كل ما يلي صحيح ما عدا:</v>
       </c>
@@ -2664,12 +2664,8 @@
       <c r="G65" t="str">
         <v>1</v>
       </c>
-      <c r="H65" t="str" xml:space="preserve">
-        <v xml:space="preserve">يصيب فقط الطرف الايمن
-بصير عندي توسع للاذينة اليمنى على حساب البطين الايمن
-التاجي مالوش دعوة
-بسبب انو توضع ثلاثي الشرف بجي منخفض
-</v>
+      <c r="H65" t="str">
+        <v>يصيب فقط الطرف الايمنبصير عندي توسع للاذينة اليمنى على حساب البطين الايمنالتاجي مالوش دعوةبسبب انو توضع ثلاثي الشرف بجي منخفض</v>
       </c>
       <c r="I65" t="str">
         <v>جراحة 2</v>
@@ -2996,7 +2992,7 @@
         <v>قلبية</v>
       </c>
     </row>
-    <row r="75" xml:space="preserve">
+    <row r="75">
       <c r="A75" t="str">
         <v>في الصمام التاجي كل ما يلي صحيح عدا:</v>
       </c>
@@ -3018,9 +3014,8 @@
       <c r="G75" t="str">
         <v>3</v>
       </c>
-      <c r="H75" t="str" xml:space="preserve">
-        <v xml:space="preserve"> تتمزق هذه الحليمة بالاحتشاء بسبب ترويتها بشريان وحيد
-</v>
+      <c r="H75" t="str">
+        <v xml:space="preserve"> تتمزق هذه الحليمة بالاحتشاء بسبب ترويتها بشريان وحيد</v>
       </c>
       <c r="I75" t="str">
         <v>جراحة 2</v>
@@ -4117,7 +4112,7 @@
         <v>قلبية</v>
       </c>
     </row>
-    <row r="107" xml:space="preserve">
+    <row r="107">
       <c r="A107" t="str">
         <v>من مضادات استطباب زرع القلب كل ما يلي صحيح عدا:</v>
       </c>
@@ -4139,9 +4134,8 @@
       <c r="G107" t="str">
         <v>4</v>
       </c>
-      <c r="H107" t="str" xml:space="preserve">
-        <v xml:space="preserve">التفسير هو حدوث استجابة التهابية شديدة
-تؤدي الى تخثر منتشر في الاوعية و ليس فرط نمو بطانة</v>
+      <c r="H107" t="str">
+        <v>التفسير هو حدوث استجابة التهابية شديدةتؤدي الى تخثر منتشر في الاوعية و ليس فرط نمو بطانة</v>
       </c>
       <c r="I107" t="str">
         <v>جراحة 2</v>
@@ -4888,7 +4882,7 @@
         <v>صدرية</v>
       </c>
     </row>
-    <row r="129" xml:space="preserve">
+    <row r="129">
       <c r="A129" t="str">
         <v>يستطب فتح الصدر الجراحي في تدمي الجنب:</v>
       </c>
@@ -4910,9 +4904,8 @@
       <c r="G129" t="str">
         <v>2</v>
       </c>
-      <c r="H129" t="str" xml:space="preserve">
-        <v xml:space="preserve">مع استرواح الصدر يعالج بتفجير الصدر بشكل مبدئي
-اذا فشل ننتقل الى الجراحي</v>
+      <c r="H129" t="str">
+        <v>مع استرواح الصدر يعالج بتفجير الصدر بشكل مبدئياذا فشل ننتقل الى الجراحي</v>
       </c>
       <c r="I129" t="str">
         <v>جراحة 2</v>
@@ -5029,7 +5022,7 @@
         <v>صدرية</v>
       </c>
     </row>
-    <row r="133" xml:space="preserve">
+    <row r="133">
       <c r="A133" t="str">
         <v>اذيات القناة الصدريه الرضيه:</v>
       </c>
@@ -5051,13 +5044,8 @@
       <c r="G133" t="str">
         <v>4</v>
       </c>
-      <c r="H133" t="str" xml:space="preserve">
-        <v xml:space="preserve">الخيار الاول الانصباب الكيلوسي (Chylothorax) يكون عادةً عكراً/لبنياً بسبب وجود الكيلوس (غني بالشحوم).  
-  لا يكون محجباً (loculated) منذ البداية، بل قد يصبح كذلك لاحقاً إذا استمر أو حدث التهاب ثانوي.  
-الخيار الثاني - العلاج المحافظ يعتمد على حمية قليلة الدسم (خصوصاً الدهون طويلة السلسلة) مع إعطاء دهون متوسطة السلسلة (MCT) لأنها تُمتص مباشرة إلى الدوران البابي ولا تمر بالقناة الصدرية.
-الخيار الثالث  ...  - العلاج يبدأ محافظاً (حمية + تصريف + دعم غذائي ± أوكتريوتيد).  
-  - الجراحة (ربط القناة الصدرية أو تحويلة) تُجرى فقط إذا فشل العلاج المحافظ أو كان التسريب غزيراً مستمراً.
-  - ليست الحمية الخالية من البروتين.  </v>
+      <c r="H133" t="str">
+        <v xml:space="preserve">الخيار الاول الانصباب الكيلوسي (Chylothorax) يكون عادةً عكراً/لبنياً بسبب وجود الكيلوس (غني بالشحوم).    لا يكون محجباً (loculated) منذ البداية، بل قد يصبح كذلك لاحقاً إذا استمر أو حدث التهاب ثانوي.  الخيار الثاني - العلاج المحافظ يعتمد على حمية قليلة الدسم (خصوصاً الدهون طويلة السلسلة) مع إعطاء دهون متوسطة السلسلة (MCT) لأنها تُمتص مباشرة إلى الدوران البابي ولا تمر بالقناة الصدرية.الخيار الثالث  ...  - العلاج يبدأ محافظاً (حمية + تصريف + دعم غذائي ± أوكتريوتيد).    - الجراحة (ربط القناة الصدرية أو تحويلة) تُجرى فقط إذا فشل العلاج المحافظ أو كان التسريب غزيراً مستمراً.    - ليست الحمية الخالية من البروتين.  </v>
       </c>
       <c r="I133" t="str">
         <v>جراحة 2</v>
@@ -5174,7 +5162,7 @@
         <v>صدرية</v>
       </c>
     </row>
-    <row r="137" xml:space="preserve">
+    <row r="137">
       <c r="A137" t="str">
         <v>اذية المري الرضية:</v>
       </c>
@@ -5196,12 +5184,8 @@
       <c r="G137" t="str">
         <v>3</v>
       </c>
-      <c r="H137" t="str" xml:space="preserve">
-        <v xml:space="preserve">طلع بالبحث اصابته صعبة لانو محمي بالقصبات
-و ممكن انظر 
-وممكن يسبب استرواح صدر
-في اكثر من اجابة صح
-معناها الها علاقة منهاج الدكتور</v>
+      <c r="H137" t="str">
+        <v>طلع بالبحث اصابته صعبة لانو محمي بالقصباتو ممكن انظر وممكن يسبب استرواح صدرفي اكثر من اجابة صحمعناها الها علاقة منهاج الدكتور</v>
       </c>
       <c r="I137" t="str">
         <v>جراحة 2</v>
@@ -5495,10 +5479,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>سؤال عن انو الدوالي باليمين اشيع (اختر الغلط)</v>
+        <v>سؤال عن الدوالي (اختر الغلط)</v>
       </c>
       <c r="B146" t="str">
-        <v>_</v>
+        <v xml:space="preserve"> باليمين اشيع</v>
       </c>
       <c r="C146" t="str">
         <v/>
@@ -5516,7 +5500,7 @@
         <v>1</v>
       </c>
       <c r="H146" t="str">
-        <v/>
+        <v xml:space="preserve"> اشيع  باليسار لانها بتصب على الوريد الكلوي</v>
       </c>
       <c r="I146" t="str">
         <v>جراحة 3</v>
@@ -5682,16 +5666,16 @@
         <v>نقص الكريات البيض</v>
       </c>
       <c r="E151" t="str">
-        <v xml:space="preserve"> نقص الكريات البيض</v>
+        <v/>
       </c>
       <c r="F151" t="str">
         <v/>
       </c>
       <c r="G151" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H151" t="str">
-        <v/>
+        <v>الدوالي باليمين</v>
       </c>
       <c r="I151" t="str">
         <v>جراحة 3</v>
@@ -5738,12 +5722,12 @@
         <v>عصبية</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" xml:space="preserve">
       <c r="A153" t="str">
         <v>ضغط البطينات شقد؟</v>
       </c>
       <c r="B153">
-        <v>1015</v>
+        <v>10-15</v>
       </c>
       <c r="C153" t="str">
         <v/>
@@ -5760,8 +5744,9 @@
       <c r="G153" t="str">
         <v>1</v>
       </c>
-      <c r="H153" t="str">
-        <v/>
+      <c r="H153" t="str" xml:space="preserve">
+        <v xml:space="preserve">من ٥ ل١٥
+او من ١٠ ل١٥ كمان مقبول</v>
       </c>
       <c r="I153" t="str">
         <v>جراحة 3</v>
@@ -5913,7 +5898,7 @@
         <v>بولية</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" xml:space="preserve">
       <c r="A158" t="str">
         <v>في سؤال عن التشوهات الوريدية الشريانية حدا متذكر السؤال وخياراته؟</v>
       </c>
@@ -5935,8 +5920,9 @@
       <c r="G158" t="str">
         <v>1</v>
       </c>
-      <c r="H158" t="str">
-        <v/>
+      <c r="H158" t="str" xml:space="preserve">
+        <v xml:space="preserve">سؤال ١٤ اذا نفس الدورات انو بيعمل اعراض عصبية بارتفاع الضغط داخل القحف او اعراض كتلة شاغلة الحيز
+وبتكون غلط</v>
       </c>
       <c r="I158" t="str">
         <v>جراحة 3</v>
@@ -6683,7 +6669,7 @@
         <v>بولية</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" xml:space="preserve">
       <c r="A180" t="str">
         <v>سؤال ورم ويلمز</v>
       </c>
@@ -6705,8 +6691,9 @@
       <c r="G180" t="str">
         <v>1</v>
       </c>
-      <c r="H180" t="str">
-        <v/>
+      <c r="H180" t="str" xml:space="preserve">
+        <v xml:space="preserve">كلن صح
+بقا الله العليم شو بدو الدكتور</v>
       </c>
       <c r="I180" t="str">
         <v>جراحة 3</v>
@@ -6811,7 +6798,7 @@
         <v>1</v>
       </c>
       <c r="H183" t="str">
-        <v/>
+        <v>هو نسيج ضام رخو</v>
       </c>
       <c r="I183" t="str">
         <v>جراحة 3</v>
@@ -7243,7 +7230,7 @@
         <v>عصبية</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" xml:space="preserve">
       <c r="A196" t="str">
         <v xml:space="preserve"> النزف تحت العنكبوتي العفوي اختر الغلط:</v>
       </c>
@@ -7265,8 +7252,16 @@
       <c r="G196" t="str">
         <v>3</v>
       </c>
-      <c r="H196" t="str">
-        <v/>
+      <c r="H196" t="str" xml:space="preserve">
+        <v xml:space="preserve">مابعرف شو الصح
+بس هاد تفسير محتمل
+:
+- النزف العنكبوتي العفوي سببه غالباً تمزق أم دم شريانية.  
+- العلاج قد يكون جراحة أو تداخل وعائي، لكن ليس دوماً جراحي فقط.  
+- الرض الشديد يسبب نزف تحت العنكبوتية رضي وليس عفوي.  
+- أشيع مكان: الدائرة الشريانية لويليس، وليس الجبهي الصدغي.  
+👉 إذن: كل العبارات المذكورة خاطئة أو غير دقيقة.
+</v>
       </c>
       <c r="I196" t="str">
         <v>جراحة 3</v>
@@ -7406,7 +7401,7 @@
         <v>4</v>
       </c>
       <c r="H200" t="str">
-        <v/>
+        <v>يقع في جذع الدماغ</v>
       </c>
       <c r="I200" t="str">
         <v>جراحة 3</v>
@@ -7890,10 +7885,10 @@
         <v>يعتبر النزف فوق الجافية أقل النزوف داخل القحف شيوعا</v>
       </c>
       <c r="F214" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G214" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H214" t="str">
         <v/>
@@ -7925,13 +7920,13 @@
         <v>تحدث غالبا عند الاطفال واليفع</v>
       </c>
       <c r="F215" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G215" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H215" t="str">
-        <v/>
+        <v>غاليا حميدة</v>
       </c>
       <c r="I215" t="str">
         <v>جراحة 3</v>
@@ -7960,13 +7955,13 @@
         <v>يعتبر الاطفال وكبار السن اكثر عرضه للاصابه بالنزف تحت الجافية</v>
       </c>
       <c r="F216" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G216" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H216" t="str">
-        <v/>
+        <v>السبب الاوردة الجسرية</v>
       </c>
       <c r="I216" t="str">
         <v>جراحة 3</v>
@@ -7978,7 +7973,7 @@
         <v>عصبية</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" xml:space="preserve">
       <c r="A217" t="str">
         <v>بالنسبه لورم غمد الليف العصب السمعي:</v>
       </c>
@@ -7995,13 +7990,25 @@
         <v>مع مرور الوقت يسبب انضغاط على الاعصاب القحفيه المجاوره( الثاني والثالث)</v>
       </c>
       <c r="F217" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G217" t="str">
-        <v>5</v>
-      </c>
-      <c r="H217" t="str">
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="H217" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+1. ورم خبيث ❌  
+- خطأ: هو ورم حميد ينشأ من خلايا شوان المغلفة للعصب الدهليزي (الفرع الدهليزي من العصب القحفي الثامن).  
+- ينمو ببطء لكنه قد يضغط على البنى المجاورة.  
+2. أشيع أورام المنطقة فوق الخيمة ❌  
+- خطأ: هو أشيع أورام الزاوية الجسرية المخيخية (Cerebellopontine angle)، أي في المنطقة تحت الخيمة (infratentorial)، وليس فوقها.  
+3. يسبب هذا الورم نقص سمع مترق مع دوار واضطراب توازن ✅  
+- صحيح: العرض الأشيع هو نقص سمع مترق أحادي الجانب (90% من الحالات)، مع طنين واضطراب توازن/دوار.  
+4. مع مرور الوقت يسبب انضغاط على الأعصاب القحفية المجاورة الثاني والثالث ❌  
+- خطأ: الأعصاب التي تتأثر بالضغط هي:  
+  - العصب الخامس (Trigeminal) → خدر/ألم وجهي.  
+  - العصب السابع (Facial) → ضعف وجهي.  
+  - الأعصاب القحفية II و III لا تتأثر عادة (هي أمامية أكثر).</v>
       </c>
       <c r="I217" t="str">
         <v>جراحة 3</v>
@@ -8030,13 +8037,13 @@
         <v>العلاج الجراحي في معظم الحالات</v>
       </c>
       <c r="F218" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G218" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H218" t="str">
-        <v/>
+        <v>يجب ان يكون محافظ</v>
       </c>
       <c r="I218" t="str">
         <v>جراحة 3</v>
@@ -8048,7 +8055,7 @@
         <v>عصبية</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" xml:space="preserve">
       <c r="A219" t="str">
         <v>فيما يخص الاورام الاروميه الوعائيه ما عدا:</v>
       </c>
@@ -8065,13 +8072,17 @@
         <v>يتم الشفاء بتفريغ الاف الكيسيه واستئصال هذه العقيده جراحيا</v>
       </c>
       <c r="F219" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G219" t="str">
-        <v>5</v>
-      </c>
-      <c r="H219" t="str">
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="H219" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+4. يتم الشفاء بتفريغ الآفة الكيسية واستئصال هذه العقيدة جراحياً ❌  
+- خطأ:  
+  - تفريغ الكيسة وحده غير كافٍ → يؤدي إلى النكس.  
+  - العلاج الشافي هو استئصال العقدة الورمية (mural nodule) كاملة، مع أو بدون الكيسة.</v>
       </c>
       <c r="I219" t="str">
         <v>جراحة 3</v>
@@ -8100,10 +8111,10 @@
         <v>عدم فتح العينين عند اي منبه عندها ياخذ المريض صفر درجه</v>
       </c>
       <c r="F220" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G220" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H220" t="str">
         <v/>
@@ -8135,13 +8146,13 @@
         <v>التكلسات نادره الحدوث في هذا الورم</v>
       </c>
       <c r="F221" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G221" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H221" t="str">
-        <v/>
+        <v>على العكس التكلسات شائعة</v>
       </c>
       <c r="I221" t="str">
         <v>جراحة 3</v>
@@ -8155,7 +8166,7 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>في تناثر ارنولد كياري نمط اول ما عدا: (الحل غير  متوفر)</v>
+        <v xml:space="preserve">في تناثر ارنولد كياري نمط اول ما عدا: </v>
       </c>
       <c r="B222" t="str">
         <v>تظهر الاعراض بعمر متاخر</v>
@@ -8173,10 +8184,10 @@
         <v>العلاج جراحي في الحالات الشديده</v>
       </c>
       <c r="G222" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H222" t="str">
-        <v/>
+        <v>تتراقق هذه الكيسة بالنمط الثاني ( القيلة السحائية النخاعية)</v>
       </c>
       <c r="I222" t="str">
         <v>جراحة 3</v>
@@ -8205,13 +8216,13 @@
         <v>اختلاطاتها نادره بالمقارنه مع العلاج الشعاعي ولا يمكن نفي حدوث وذمه دماغيه كاختلاط</v>
       </c>
       <c r="F223" t="str">
-        <v>الحل غير متوفر</v>
+        <v/>
       </c>
       <c r="G223" t="str">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H223" t="str">
-        <v/>
+        <v>الاورام الصغير اصغر من ٣ سم</v>
       </c>
       <c r="I223" t="str">
         <v>جراحة 3</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 06/10/2025, 11:59:15
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -8802,7 +8802,7 @@
         <v>عظمية</v>
       </c>
     </row>
-    <row r="241" xml:space="preserve">
+    <row r="241">
       <c r="A241" t="str">
         <v>الخراخر عالية الصوت بمريض كرب تنفسي ARDS يعني:</v>
       </c>
@@ -8824,9 +8824,8 @@
       <c r="G241" t="str">
         <v>3</v>
       </c>
-      <c r="H241" t="str" xml:space="preserve">
-        <v xml:space="preserve">مرحلة ٣ كمان يمكن غلط بدها حدا يتأكد شو بدو المقرر 
-حسب مصادر فهو مرحلة ١</v>
+      <c r="H241" t="str">
+        <v>مرحلة ٣ كمان يمكن غلط بدها حدا يتأكد شو بدو المقرر حسب مصادر فهو مرحلة ١</v>
       </c>
       <c r="I241" t="str">
         <v>جراحة 4</v>
@@ -9243,7 +9242,7 @@
         <v>A+B+C</v>
       </c>
       <c r="G253" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H253" t="str">
         <v>ايوينغ منشؤه من النيزوديرم</v>
@@ -9643,7 +9642,7 @@
         <v>عظمية</v>
       </c>
     </row>
-    <row r="265" xml:space="preserve">
+    <row r="265">
       <c r="A265" t="str">
         <v>نجد بتناذر Albrigt McCun:</v>
       </c>
@@ -9665,10 +9664,8 @@
       <c r="G265" t="str">
         <v>5</v>
       </c>
-      <c r="H265" t="str" xml:space="preserve">
-        <v xml:space="preserve">فرط نشاط جارات الدرق: غير شائع ولا يُعد عرضاً أساسيا للمتلازمة؛ الاضطرابات الأكثر شيوعاً هي فرط نشاط الدرق، وفرط هرمونات أخرى مثل النمو أو الكورتيزول، لكن جارات الدرق أقل حدوثاً بكثير أو نادر جداً��.الإجابة الصحيحة:
-A+B+C
-كل من "بقع جلدية قهوة بحليب" + "بلوغ جنسي مبكر" هي السمة الثلاثية الكلاسيكية، أما فرط نشاط جارات الدرق فهو عرض نادر لكنه قد يظهر ضمن طيف الاضطرابات الصماوية للمتلازمة�����.لكن حسب الكتب الطبية، الأكثر شيوعاً هو A+B فقط، بينما C (فرط نشاط جارات الدرق) غير أساسي وغالباً غير موجود عند أغلب المرضى.إذن:الجواب الأكثر دقة بحسب الكتب: A+B (بقع جلدية قهوة بحليب + بلوغ جنسي مبكر)���.</v>
+      <c r="H265" t="str">
+        <v>فرط نشاط جارات الدرق: غير شائع ولا يُعد عرضاً أساسيا للمتلازمة؛ الاضطرابات الأكثر شيوعاً هي فرط نشاط الدرق، وفرط هرمونات أخرى مثل النمو أو الكورتيزول، لكن جارات الدرق أقل حدوثاً بكثير أو نادر جداً��.الإجابة الصحيحة:A+B+Cكل من "بقع جلدية قهوة بحليب" + "بلوغ جنسي مبكر" هي السمة الثلاثية الكلاسيكية، أما فرط نشاط جارات الدرق فهو عرض نادر لكنه قد يظهر ضمن طيف الاضطرابات الصماوية للمتلازمة�����.لكن حسب الكتب الطبية، الأكثر شيوعاً هو A+B فقط، بينما C (فرط نشاط جارات الدرق) غير أساسي وغالباً غير موجود عند أغلب المرضى.إذن:الجواب الأكثر دقة بحسب الكتب: A+B (بقع جلدية قهوة بحليب + بلوغ جنسي مبكر)���.</v>
       </c>
       <c r="I265" t="str">
         <v>جراحة 4</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 06/10/2025, 12:29:37
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -8052,7 +8052,7 @@
         <v/>
       </c>
       <c r="G219" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H219" t="str">
         <v>_x000d_4. يتم الشفاء بتفريغ الآفة الكيسية واستئصال هذه العقيدة جراحياً ❌  _x000d_ خطأ:  _x000d_   تفريغ الكيسة وحده غير كافٍ → يؤدي إلى النكس.  _x000d_   العلاج الشافي هو استئصال العقدة الورمية (mural nodule) كاملة، مع أو بدون الكيسة.</v>
@@ -9592,7 +9592,7 @@
         <v>AUTOGRAFT</v>
       </c>
       <c r="G263" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H263" t="str">
         <v/>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 06/10/2025, 12:39:32
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -8437,10 +8437,10 @@
         <v>A+B+C</v>
       </c>
       <c r="G230" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H230" t="str">
-        <v/>
+        <v>اذا اختر الغلط: A... اذا اختر الصحE</v>
       </c>
       <c r="I230" t="str">
         <v>جراحة 4</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 06/10/2025, 16:25:59
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -4135,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="H107" t="str">
-        <v>التفسير هو حدوث استجابة التهابية شديدةتؤدي الى تخثر منتشر في الاوعية و ليس فرط نمو بطانة</v>
+        <v/>
       </c>
       <c r="I107" t="str">
         <v>جراحة 2</v>
@@ -4205,7 +4205,7 @@
         <v>1</v>
       </c>
       <c r="H109" t="str">
-        <v>الورم المذكور سليم</v>
+        <v>التفسير هو حدوث استجابة التهابية شديدةتؤدي الى تخثر منتشر في الاوعية و ليس فرط نمو بطانة</v>
       </c>
       <c r="I109" t="str">
         <v>جراحة 2</v>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 10/6/2025, 5:53:53 PM
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -8612,7 +8612,7 @@
         <v>نقرس</v>
       </c>
       <c r="G235" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H235" t="str">
         <v/>
@@ -9137,7 +9137,7 @@
         <v>A+B+C</v>
       </c>
       <c r="G250" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H250" t="str">
         <v/>
@@ -10957,7 +10957,7 @@
         <v>داء كارولي</v>
       </c>
       <c r="G302" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H302" t="str">
         <v/>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 10/10/2025, 16:24:42
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -23431,7 +23431,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K658" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="659">
@@ -23501,7 +23501,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K660" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="661">
@@ -23536,7 +23536,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K661" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="662">
@@ -23571,7 +23571,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K662" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="663">
@@ -23606,7 +23606,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K663" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="664">
@@ -23641,7 +23641,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K664" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="665">
@@ -23676,7 +23676,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K665" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="666">
@@ -23711,7 +23711,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K666" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="667">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 10/10/2025, 22:13:11
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -22941,7 +22941,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K644" t="str">
-        <v/>
+        <v>الملتحمة</v>
       </c>
     </row>
     <row r="645">
@@ -23276,7 +23276,7 @@
         <v>حكة</v>
       </c>
       <c r="F654" t="str">
-        <v>وجود كليبات ملتحمية</v>
+        <v>وجود جريبات ملتحمية</v>
       </c>
       <c r="G654" t="str">
         <v>4</v>
@@ -23291,7 +23291,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K654" t="str">
-        <v/>
+        <v>الملتحمة</v>
       </c>
     </row>
     <row r="655">
@@ -23326,7 +23326,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K655" t="str">
-        <v/>
+        <v>الملتحمة</v>
       </c>
     </row>
     <row r="656">
@@ -23361,7 +23361,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K656" t="str">
-        <v/>
+        <v>الملتحمة</v>
       </c>
     </row>
     <row r="657">
@@ -23396,7 +23396,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K657" t="str">
-        <v/>
+        <v>الملتحمة</v>
       </c>
     </row>
     <row r="658">
@@ -23921,7 +23921,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K672" t="str">
-        <v/>
+        <v>الملتحمة</v>
       </c>
     </row>
     <row r="673">
@@ -24586,7 +24586,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K691" t="str">
-        <v/>
+        <v>الاجفان</v>
       </c>
     </row>
     <row r="692">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 10/10/2025, 23:22:50
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -23081,7 +23081,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K648" t="str">
-        <v/>
+        <v>جهاز الدمع</v>
       </c>
     </row>
     <row r="649">
@@ -23221,7 +23221,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K652" t="str">
-        <v/>
+        <v>جهاز الدمع</v>
       </c>
     </row>
     <row r="653">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 11/10/2025, 00:17:23
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -23256,7 +23256,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K653" t="str">
-        <v/>
+        <v>جهاز الدمع</v>
       </c>
     </row>
     <row r="654">
@@ -24854,7 +24854,7 @@
         <v xml:space="preserve"> تشوه ابيشتاين لمثلث الشرف</v>
       </c>
       <c r="G699">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H699" t="str">
         <v/>

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 11/10/2025, 01:58:20
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -22976,7 +22976,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K645" t="str">
-        <v/>
+        <v>الحول</v>
       </c>
     </row>
     <row r="646">
@@ -23116,7 +23116,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K649" t="str">
-        <v/>
+        <v>الحول</v>
       </c>
     </row>
     <row r="650">
@@ -23151,7 +23151,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K650" t="str">
-        <v/>
+        <v>الحول</v>
       </c>
     </row>
     <row r="651">
@@ -23186,7 +23186,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K651" t="str">
-        <v/>
+        <v>الحول</v>
       </c>
     </row>
     <row r="652">
@@ -23466,7 +23466,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K659" t="str">
-        <v/>
+        <v>الحول</v>
       </c>
     </row>
     <row r="660">
@@ -24656,7 +24656,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K693" t="str">
-        <v/>
+        <v>الحول</v>
       </c>
     </row>
     <row r="694">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 11/10/2025, 23:45:20
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -22241,7 +22241,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K624" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="625">
@@ -22276,7 +22276,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K625" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="626">
@@ -22311,7 +22311,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K626" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="627">
@@ -22346,7 +22346,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K627" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="628">
@@ -22381,7 +22381,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K628" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="629">
@@ -22416,7 +22416,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K629" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="630">
@@ -22451,7 +22451,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K630" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="631">
@@ -22486,7 +22486,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K631" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="632">
@@ -22521,7 +22521,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K632" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="633">
@@ -22556,7 +22556,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K633" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="634">
@@ -22591,7 +22591,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K634" t="str">
-        <v/>
+        <v>الشبكية والزجاجي</v>
       </c>
     </row>
     <row r="635">

</xml_diff>

<commit_message>
WAY Corrector - تحديث الملف: 12/10/2025, 22:51:35
</commit_message>
<xml_diff>
--- a/MCQD.xlsx
+++ b/MCQD.xlsx
@@ -22066,7 +22066,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K619" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="620">
@@ -22101,7 +22101,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K620" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="621">
@@ -22136,7 +22136,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K621" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="622">
@@ -22171,7 +22171,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K622" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="623">
@@ -22206,7 +22206,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K623" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="624">
@@ -22626,7 +22626,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K635" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="636">
@@ -22661,7 +22661,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K636" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="637">
@@ -22696,7 +22696,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K637" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="638">
@@ -22731,7 +22731,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K638" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="639">
@@ -22766,7 +22766,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K639" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="640">
@@ -22801,7 +22801,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K640" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="641">
@@ -22836,7 +22836,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K641" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="642">
@@ -22871,7 +22871,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K642" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="643">
@@ -22906,7 +22906,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K643" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="644">
@@ -23011,7 +23011,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K646" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="647">
@@ -23046,7 +23046,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K647" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="648">
@@ -23746,7 +23746,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K667" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="668">
@@ -23781,7 +23781,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K668" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="669">
@@ -23816,7 +23816,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K669" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="670">
@@ -23851,7 +23851,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K670" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="671">
@@ -23886,7 +23886,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K671" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="672">
@@ -23956,7 +23956,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K673" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="674">
@@ -23991,7 +23991,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K674" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="675">
@@ -24026,7 +24026,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K675" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="676">
@@ -24061,7 +24061,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K676" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="677">
@@ -24096,7 +24096,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K677" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="678">
@@ -24131,7 +24131,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K678" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="679">
@@ -24166,7 +24166,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K679" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="680">
@@ -24201,7 +24201,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K680" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="681">
@@ -24236,7 +24236,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K681" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="682">
@@ -24271,7 +24271,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K682" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="683">
@@ -24306,7 +24306,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K683" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="684">
@@ -24341,7 +24341,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K684" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="685">
@@ -24376,7 +24376,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K685" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="686">
@@ -24411,7 +24411,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K686" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="687">
@@ -24446,7 +24446,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K687" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="688">
@@ -24481,7 +24481,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K688" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="689">
@@ -24516,7 +24516,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K689" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="690">
@@ -24551,7 +24551,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K690" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="691">
@@ -24691,7 +24691,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K694" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="695">
@@ -24726,7 +24726,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K695" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="696">
@@ -24761,7 +24761,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K696" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="697">
@@ -24796,7 +24796,7 @@
         <v>الفصل الثاني 2024-2025</v>
       </c>
       <c r="K697" t="str">
-        <v/>
+        <v>أُخرى</v>
       </c>
     </row>
     <row r="698">

</xml_diff>